<commit_message>
Added Hands On - Day 1 .
</commit_message>
<xml_diff>
--- a/Java 8 & 11 - TOC.xlsx
+++ b/Java 8 & 11 - TOC.xlsx
@@ -767,10 +767,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -859,7 +859,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -867,9 +874,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -881,25 +888,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -919,25 +910,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -957,8 +941,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -966,14 +951,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1013,13 +1013,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1031,19 +1043,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1067,55 +1079,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1127,13 +1097,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1145,43 +1109,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1194,6 +1122,78 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1275,21 +1275,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1328,26 +1313,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1371,18 +1336,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1395,127 +1395,127 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1997,9 +1997,9 @@
   <dimension ref="A1:E128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -2316,7 +2316,7 @@
       <c r="B48" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="9" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2842,7 +2842,7 @@
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="2. Module Outline"/>
     <hyperlink ref="B31" r:id="rId2" display="16. New Patterns: The Predicate Interface Example"/>
-    <hyperlink ref="C15" r:id="rId3" display="https://www.hackerrank.com/challenges/java-lambda-expressions/problem"/>
+    <hyperlink ref="C15" r:id="rId3" display="https://www.hackerrank.com/challenges/java-lambda-expressions/problem" tooltip="https://www.hackerrank.com/challenges/java-lambda-expressions/problem"/>
     <hyperlink ref="C16" r:id="rId4" display="https://www.hackerrank.com/challenges/dynamic-array/problem" tooltip="https://www.hackerrank.com/challenges/dynamic-array/problem"/>
     <hyperlink ref="C23" r:id="rId5" display="https://www.hackerrank.com/challenges/array-left-rotation" tooltip="https://www.hackerrank.com/challenges/array-left-rotation"/>
     <hyperlink ref="C22" r:id="rId6" display="https://www.hackerrank.com/challenges/sparse-arrays/problem" tooltip="https://www.hackerrank.com/challenges/sparse-arrays/problem"/>

</xml_diff>

<commit_message>
Added Course Materials -  Day 2 .
</commit_message>
<xml_diff>
--- a/Java 8 & 11 - TOC.xlsx
+++ b/Java 8 & 11 - TOC.xlsx
@@ -767,10 +767,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -872,14 +872,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -887,10 +879,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -941,9 +934,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -958,22 +966,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -985,8 +978,15 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -996,6 +996,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1013,13 +1019,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1031,31 +1037,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1079,7 +1091,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1091,49 +1163,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1145,55 +1187,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1274,17 +1280,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1328,11 +1328,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1354,15 +1360,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1371,18 +1368,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1395,131 +1401,131 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1555,37 +1561,43 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1932,56 +1944,56 @@
   <sheetData>
     <row r="7" ht="13.5"/>
     <row r="8" ht="13.5" spans="6:9">
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="6:9">
-      <c r="F9" s="21">
+      <c r="F9" s="25">
         <v>1</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="27">
         <v>5</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="27">
         <v>20</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="6:9">
-      <c r="F10" s="24">
+      <c r="F10" s="28">
         <v>2</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="27">
         <v>5</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="27">
         <v>20</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="6:9">
-      <c r="F11" s="26"/>
-      <c r="G11" s="27" t="s">
+      <c r="F11" s="30"/>
+      <c r="G11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="H11" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="28" t="s">
+      <c r="I11" s="32" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1997,9 +2009,9 @@
   <dimension ref="A1:E128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -2030,79 +2042,79 @@
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" ht="15" spans="1:2">
       <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" ht="15" spans="1:2">
       <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:2">
       <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:2">
       <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:2">
       <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:2">
       <c r="A9" s="4"/>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:2">
       <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:2">
       <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:2">
       <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:2">
       <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="1" ht="15" spans="1:2">
       <c r="A14" s="4"/>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="16" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="1" ht="30" spans="1:3">
       <c r="A15" s="4"/>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -2111,7 +2123,7 @@
     </row>
     <row r="16" customFormat="1" ht="30" spans="1:3">
       <c r="A16" s="4"/>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="17" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -2150,7 +2162,7 @@
     </row>
     <row r="22" customFormat="1" ht="30" spans="1:3">
       <c r="A22" s="4"/>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="18" t="s">
         <v>35</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -2159,7 +2171,7 @@
     </row>
     <row r="23" customFormat="1" ht="30" spans="1:3">
       <c r="A23" s="4"/>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="18" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -2168,7 +2180,7 @@
     </row>
     <row r="24" customFormat="1" ht="30" spans="1:3">
       <c r="A24" s="4"/>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="18" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -2189,119 +2201,121 @@
       <c r="A27" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" customFormat="1" ht="15" spans="1:2">
       <c r="A28" s="4"/>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" customFormat="1" ht="15" spans="1:2">
       <c r="A29" s="4"/>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="30" customFormat="1" ht="15" spans="1:3">
       <c r="A30" s="4"/>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="17"/>
+      <c r="C30" s="20"/>
     </row>
     <row r="31" customFormat="1" ht="15" spans="1:2">
       <c r="A31" s="4"/>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="19" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="32" customFormat="1" ht="15" spans="1:2">
       <c r="A32" s="4"/>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="19" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="33" customFormat="1" ht="15" spans="1:2">
       <c r="A33" s="4"/>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="19" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="34" customFormat="1" ht="15" spans="1:2">
       <c r="A34" s="4"/>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" ht="8" customHeight="1"/>
+    <row r="35" ht="8" customHeight="1" spans="2:2">
+      <c r="B35" s="21"/>
+    </row>
     <row r="36" customFormat="1" ht="15" spans="1:2">
       <c r="A36" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="19" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="37" customFormat="1" ht="15" spans="1:2">
       <c r="A37" s="4"/>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="19" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="38" customFormat="1" ht="15" spans="1:2">
       <c r="A38" s="4"/>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="19" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="39" customFormat="1" ht="15" spans="1:2">
       <c r="A39" s="4"/>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="40" customFormat="1" ht="15" spans="1:2">
       <c r="A40" s="4"/>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="19" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="41" customFormat="1" ht="15" spans="1:2">
       <c r="A41" s="4"/>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="19" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="42" customFormat="1" ht="15" spans="1:2">
       <c r="A42" s="4"/>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="19" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="43" customFormat="1" ht="15" spans="1:2">
       <c r="A43" s="4"/>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="44" customFormat="1" ht="15" spans="1:2">
       <c r="A44" s="4"/>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="19" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="45" customFormat="1" ht="15" spans="1:2">
       <c r="A45" s="4"/>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="19" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="46" customFormat="1" ht="15" spans="1:2">
       <c r="A46" s="4"/>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="19" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2313,7 +2327,7 @@
     </row>
     <row r="48" ht="30" spans="1:3">
       <c r="A48" s="4"/>
-      <c r="B48" t="s">
+      <c r="B48" s="21" t="s">
         <v>63</v>
       </c>
       <c r="C48" s="9" t="s">
@@ -2322,7 +2336,7 @@
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="4"/>
-      <c r="B49" t="s">
+      <c r="B49" s="21" t="s">
         <v>65</v>
       </c>
       <c r="C49" s="7"/>
@@ -2639,7 +2653,7 @@
       <c r="B99" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C99" s="18" t="s">
+      <c r="C99" s="22" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2679,7 +2693,7 @@
       <c r="B105" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C105" s="18" t="s">
+      <c r="C105" s="22" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Course Materials -  Day 3 .
</commit_message>
<xml_diff>
--- a/Java 8 & 11 - TOC.xlsx
+++ b/Java 8 & 11 - TOC.xlsx
@@ -768,9 +768,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -865,10 +865,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -879,17 +880,77 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -910,40 +971,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -956,37 +985,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -996,12 +996,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1019,19 +1013,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1043,13 +1031,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1067,7 +1067,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1079,13 +1097,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1097,31 +1157,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1139,67 +1175,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1289,17 +1283,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1314,16 +1302,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1344,15 +1332,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1368,164 +1371,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1561,43 +1555,42 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1944,56 +1937,56 @@
   <sheetData>
     <row r="7" ht="13.5"/>
     <row r="8" ht="13.5" spans="6:9">
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="23" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="6:9">
-      <c r="F9" s="25">
+      <c r="F9" s="24">
         <v>1</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="26">
         <v>5</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="26">
         <v>20</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="6:9">
-      <c r="F10" s="28">
+      <c r="F10" s="27">
         <v>2</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10" s="26">
         <v>5</v>
       </c>
-      <c r="I10" s="27">
+      <c r="I10" s="26">
         <v>20</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="6:9">
-      <c r="F11" s="30"/>
-      <c r="G11" s="31" t="s">
+      <c r="F11" s="29"/>
+      <c r="G11" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="32" t="s">
+      <c r="I11" s="31" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2009,9 +2002,9 @@
   <dimension ref="A1:E128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35:B46"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -2201,121 +2194,121 @@
       <c r="A27" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="15" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" customFormat="1" ht="15" spans="1:2">
       <c r="A28" s="4"/>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="15" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" customFormat="1" ht="15" spans="1:2">
       <c r="A29" s="4"/>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="15" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="30" customFormat="1" ht="15" spans="1:3">
       <c r="A30" s="4"/>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="20"/>
+      <c r="C30" s="19"/>
     </row>
     <row r="31" customFormat="1" ht="15" spans="1:2">
       <c r="A31" s="4"/>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="15" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="32" customFormat="1" ht="15" spans="1:2">
       <c r="A32" s="4"/>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="33" customFormat="1" ht="15" spans="1:2">
       <c r="A33" s="4"/>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="34" customFormat="1" ht="15" spans="1:2">
       <c r="A34" s="4"/>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="15" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="35" ht="8" customHeight="1" spans="2:2">
-      <c r="B35" s="21"/>
+      <c r="B35" s="20"/>
     </row>
     <row r="36" customFormat="1" ht="15" spans="1:2">
       <c r="A36" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="15" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="37" customFormat="1" ht="15" spans="1:2">
       <c r="A37" s="4"/>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="15" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="38" customFormat="1" ht="15" spans="1:2">
       <c r="A38" s="4"/>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="15" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="39" customFormat="1" ht="15" spans="1:2">
       <c r="A39" s="4"/>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="15" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="40" customFormat="1" ht="15" spans="1:2">
       <c r="A40" s="4"/>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="41" customFormat="1" ht="15" spans="1:2">
       <c r="A41" s="4"/>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="42" customFormat="1" ht="15" spans="1:2">
       <c r="A42" s="4"/>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="43" customFormat="1" ht="15" spans="1:2">
       <c r="A43" s="4"/>
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="44" customFormat="1" ht="15" spans="1:2">
       <c r="A44" s="4"/>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="45" customFormat="1" ht="15" spans="1:2">
       <c r="A45" s="4"/>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="46" customFormat="1" ht="15" spans="1:2">
       <c r="A46" s="4"/>
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="15" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2327,7 +2320,7 @@
     </row>
     <row r="48" ht="30" spans="1:3">
       <c r="A48" s="4"/>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="20" t="s">
         <v>63</v>
       </c>
       <c r="C48" s="9" t="s">
@@ -2336,7 +2329,7 @@
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="4"/>
-      <c r="B49" s="21" t="s">
+      <c r="B49" s="20" t="s">
         <v>65</v>
       </c>
       <c r="C49" s="7"/>
@@ -2653,7 +2646,7 @@
       <c r="B99" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C99" s="22" t="s">
+      <c r="C99" s="21" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2693,7 +2686,7 @@
       <c r="B105" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C105" s="22" t="s">
+      <c r="C105" s="21" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Hands On Demos - Day 3.
</commit_message>
<xml_diff>
--- a/Java 8 & 11 - TOC.xlsx
+++ b/Java 8 & 11 - TOC.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="259">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -141,6 +141,12 @@
     <t>https://www.hackerrank.com/challenges/java-loops-i/problem</t>
   </si>
   <si>
+    <t>HackerRank Assessments</t>
+  </si>
+  <si>
+    <t>Minimum Start Value</t>
+  </si>
+  <si>
     <t>Day 2</t>
   </si>
   <si>
@@ -231,6 +237,9 @@
     <t>Array Manipulation</t>
   </si>
   <si>
+    <t>The Largest String</t>
+  </si>
+  <si>
     <t>Day 3</t>
   </si>
   <si>
@@ -309,6 +318,24 @@
     <t>Frequency Queries</t>
   </si>
   <si>
+    <t>Conference Schedule</t>
+  </si>
+  <si>
+    <t>FizzBuzz</t>
+  </si>
+  <si>
+    <t>Programming Contest</t>
+  </si>
+  <si>
+    <t>Reverse Array Queries</t>
+  </si>
+  <si>
+    <t>Sort the Summary</t>
+  </si>
+  <si>
+    <t>String Reduction</t>
+  </si>
+  <si>
     <t>Day 4</t>
   </si>
   <si>
@@ -427,6 +454,12 @@
   </si>
   <si>
     <t>Common Child</t>
+  </si>
+  <si>
+    <t>Aladdin and his Carpet</t>
+  </si>
+  <si>
+    <t>Slot Machine 2.0</t>
   </si>
   <si>
     <t>Day 6</t>
@@ -768,9 +801,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -859,22 +892,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -882,22 +900,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -912,29 +914,43 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -943,14 +959,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -971,10 +979,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1013,7 +1046,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1025,7 +1160,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1037,43 +1172,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1085,109 +1220,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1277,26 +1310,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1331,21 +1346,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1363,6 +1363,39 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1374,7 +1407,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1395,131 +1428,131 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1555,20 +1588,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1937,56 +1968,56 @@
   <sheetData>
     <row r="7" ht="13.5"/>
     <row r="8" ht="13.5" spans="6:9">
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="6:9">
-      <c r="F9" s="24">
+      <c r="F9" s="22">
         <v>1</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="24">
         <v>5</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="24">
         <v>20</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="6:9">
-      <c r="F10" s="27">
+      <c r="F10" s="25">
         <v>2</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="24">
         <v>5</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10" s="24">
         <v>20</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="6:9">
-      <c r="F11" s="29"/>
-      <c r="G11" s="30" t="s">
+      <c r="F11" s="27"/>
+      <c r="G11" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="29" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1999,12 +2030,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:B13"/>
+      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -2035,79 +2066,79 @@
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" ht="15" spans="1:2">
       <c r="A4" s="4"/>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" ht="15" spans="1:2">
       <c r="A5" s="4"/>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:2">
       <c r="A6" s="4"/>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:2">
       <c r="A7" s="4"/>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:2">
       <c r="A8" s="4"/>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:2">
       <c r="A9" s="4"/>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:2">
       <c r="A10" s="4"/>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:2">
       <c r="A11" s="4"/>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:2">
       <c r="A12" s="4"/>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:2">
       <c r="A13" s="4"/>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="1" ht="15" spans="1:2">
       <c r="A14" s="4"/>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="1" ht="30" spans="1:3">
       <c r="A15" s="4"/>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -2116,7 +2147,7 @@
     </row>
     <row r="16" customFormat="1" ht="30" spans="1:3">
       <c r="A16" s="4"/>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -2155,7 +2186,7 @@
     </row>
     <row r="22" customFormat="1" ht="30" spans="1:3">
       <c r="A22" s="4"/>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="17" t="s">
         <v>35</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -2164,7 +2195,7 @@
     </row>
     <row r="23" customFormat="1" ht="30" spans="1:3">
       <c r="A23" s="4"/>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="17" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -2173,652 +2204,650 @@
     </row>
     <row r="24" customFormat="1" ht="30" spans="1:3">
       <c r="A24" s="4"/>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="17" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" customFormat="1" spans="1:2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-    </row>
-    <row r="26" ht="24.75" spans="1:2">
-      <c r="A26" s="3" t="s">
+    <row r="25" customFormat="1" ht="18" spans="1:3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" customFormat="1" ht="15" spans="1:2">
-      <c r="A27" s="4" t="s">
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" customFormat="1" ht="18" spans="1:3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" customFormat="1" spans="1:2">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+    </row>
+    <row r="28" ht="24.75" spans="1:2">
+      <c r="A28" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" customFormat="1" ht="15" spans="1:2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" customFormat="1" ht="15" spans="1:2">
+      <c r="A29" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" customFormat="1" ht="15" spans="1:2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" customFormat="1" ht="15" spans="1:3">
+    <row r="30" customFormat="1" ht="15" spans="1:2">
       <c r="A30" s="4"/>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="19"/>
     </row>
     <row r="31" customFormat="1" ht="15" spans="1:2">
       <c r="A31" s="4"/>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" customFormat="1" ht="15" spans="1:2">
+    <row r="32" customFormat="1" ht="15" spans="1:3">
       <c r="A32" s="4"/>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="C32" s="18"/>
     </row>
     <row r="33" customFormat="1" ht="15" spans="1:2">
       <c r="A33" s="4"/>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="34" customFormat="1" ht="15" spans="1:2">
       <c r="A34" s="4"/>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" ht="8" customHeight="1" spans="2:2">
-      <c r="B35" s="20"/>
+    <row r="35" customFormat="1" ht="15" spans="1:2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="36" customFormat="1" ht="15" spans="1:2">
-      <c r="A36" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="15" t="s">
+      <c r="A36" s="4"/>
+      <c r="B36" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="37" customFormat="1" ht="15" spans="1:2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="15" t="s">
+    <row r="37" ht="8" customHeight="1" spans="2:2">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" customFormat="1" ht="15" spans="1:2">
+      <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" customFormat="1" ht="15" spans="1:2">
-      <c r="A38" s="4"/>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="39" customFormat="1" ht="15" spans="1:2">
       <c r="A39" s="4"/>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="40" customFormat="1" ht="15" spans="1:2">
       <c r="A40" s="4"/>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="41" customFormat="1" ht="15" spans="1:2">
       <c r="A41" s="4"/>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="42" customFormat="1" ht="15" spans="1:2">
       <c r="A42" s="4"/>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="43" customFormat="1" ht="15" spans="1:2">
       <c r="A43" s="4"/>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="44" customFormat="1" ht="15" spans="1:2">
       <c r="A44" s="4"/>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="45" customFormat="1" ht="15" spans="1:2">
       <c r="A45" s="4"/>
-      <c r="B45" s="15" t="s">
-        <v>23</v>
+      <c r="B45" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="46" customFormat="1" ht="15" spans="1:2">
       <c r="A46" s="4"/>
-      <c r="B46" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" ht="15" spans="1:2">
+      <c r="B46" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" customFormat="1" ht="15" spans="1:2">
       <c r="A47" s="4"/>
-      <c r="B47" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="48" ht="30" spans="1:3">
+      <c r="B47" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" customFormat="1" ht="15" spans="1:2">
       <c r="A48" s="4"/>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="9" t="s">
+    </row>
+    <row r="49" ht="15" spans="1:2">
+      <c r="A49" s="4"/>
+      <c r="B49" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="49" ht="15" spans="1:3">
-      <c r="A49" s="4"/>
-      <c r="B49" s="20" t="s">
+    <row r="50" ht="30" spans="1:3">
+      <c r="A50" s="4"/>
+      <c r="B50" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="7"/>
-    </row>
-    <row r="50" ht="15" spans="1:3">
-      <c r="A50" s="4"/>
-      <c r="B50" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C50" s="7"/>
+      <c r="C50" s="9" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="51" ht="15" spans="1:3">
       <c r="A51" s="4"/>
-      <c r="B51" s="5" t="s">
-        <v>66</v>
+      <c r="B51" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="C51" s="7"/>
     </row>
     <row r="52" ht="15" spans="1:3">
       <c r="A52" s="4"/>
-      <c r="B52" s="5" t="s">
-        <v>67</v>
+      <c r="B52" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="C52" s="7"/>
     </row>
-    <row r="53" ht="15" spans="1:2">
+    <row r="53" ht="15" spans="1:3">
       <c r="A53" s="4"/>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="54" ht="30" spans="1:3">
+      <c r="C53" s="7"/>
+    </row>
+    <row r="54" ht="15" spans="1:3">
       <c r="A54" s="4"/>
-      <c r="B54" t="s">
+      <c r="B54" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" ht="15" spans="1:3">
+      <c r="C54" s="7"/>
+    </row>
+    <row r="55" ht="15" spans="1:2">
       <c r="A55" s="4"/>
-      <c r="B55" t="s">
+      <c r="B55" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="7"/>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-    </row>
-    <row r="57" ht="24.75" spans="1:2">
-      <c r="A57" s="3" t="s">
+    </row>
+    <row r="56" ht="30" spans="1:3">
+      <c r="A56" s="4"/>
+      <c r="B56" t="s">
         <v>71</v>
       </c>
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" ht="15" spans="1:2">
-      <c r="A58" s="4" t="s">
+      <c r="C56" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" ht="15" spans="1:3">
+      <c r="A57" s="4"/>
+      <c r="B57" t="s">
         <v>72</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="C57" s="7"/>
+    </row>
+    <row r="58" ht="18" spans="1:3">
+      <c r="A58" s="4"/>
+      <c r="B58" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C58" s="7"/>
+    </row>
+    <row r="59" ht="18" spans="1:3">
+      <c r="A59" s="4"/>
+      <c r="B59" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="59" ht="15" spans="1:2">
-      <c r="A59" s="4"/>
-      <c r="B59" s="5" t="s">
+      <c r="C59" s="7"/>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
+    </row>
+    <row r="61" ht="24.75" spans="1:2">
+      <c r="A61" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="60" ht="15" spans="1:2">
-      <c r="A60" s="4"/>
-      <c r="B60" s="5" t="s">
+      <c r="B61" s="3"/>
+    </row>
+    <row r="62" ht="15" spans="1:2">
+      <c r="A62" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="61" ht="15" spans="1:2">
-      <c r="A61" s="4"/>
-      <c r="B61" s="5" t="s">
+      <c r="B62" s="5" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="62" ht="15" spans="1:2">
-      <c r="A62" s="4"/>
-      <c r="B62" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="63" ht="15" spans="1:2">
       <c r="A63" s="4"/>
       <c r="B63" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" ht="15" spans="1:2">
       <c r="A64" s="4"/>
       <c r="B64" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" ht="15" spans="1:2">
       <c r="A65" s="4"/>
       <c r="B65" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" ht="15" spans="1:2">
       <c r="A66" s="4"/>
       <c r="B66" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67" ht="15" spans="1:2">
       <c r="A67" s="4"/>
       <c r="B67" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" ht="15" spans="1:2">
       <c r="A68" s="4"/>
       <c r="B68" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" ht="15" spans="1:2">
       <c r="A69" s="4"/>
       <c r="B69" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" ht="15" spans="1:2">
       <c r="A70" s="4"/>
       <c r="B70" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" ht="15" spans="1:2">
       <c r="A71" s="4"/>
       <c r="B71" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" ht="15" spans="1:2">
       <c r="A72" s="4"/>
       <c r="B72" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" ht="15" spans="1:2">
       <c r="A73" s="4"/>
       <c r="B73" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" ht="15" spans="1:2">
       <c r="A74" s="4"/>
-      <c r="B74" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="75" ht="30" spans="1:3">
+      <c r="B74" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" ht="15" spans="1:2">
       <c r="A75" s="4"/>
-      <c r="B75" t="s">
+      <c r="B75" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C75" s="7" t="s">
+    </row>
+    <row r="76" ht="15" spans="1:2">
+      <c r="A76" s="4"/>
+      <c r="B76" s="5" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="4"/>
-      <c r="B76" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="77" ht="15" spans="1:2">
       <c r="A77" s="4"/>
-      <c r="B77" s="6" t="s">
-        <v>30</v>
+      <c r="B77" s="5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="78" ht="15" spans="1:2">
       <c r="A78" s="4"/>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" ht="30" spans="1:3">
+      <c r="A79" s="4"/>
+      <c r="B79" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="79" ht="15" spans="1:2">
-      <c r="A79" s="4"/>
-      <c r="B79" s="5" t="s">
+      <c r="C79" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="80" ht="15" spans="1:2">
+    <row r="80" spans="1:2">
       <c r="A80" s="4"/>
-      <c r="B80" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="81" ht="30" spans="1:3">
+      <c r="B80" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" ht="15" spans="1:2">
       <c r="A81" s="4"/>
-      <c r="B81" t="s">
-        <v>94</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="B81" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="82" ht="15" spans="1:2">
       <c r="A82" s="4"/>
-      <c r="B82" t="s">
+      <c r="B82" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" ht="15" spans="1:2">
       <c r="A83" s="4"/>
-      <c r="B83" t="s">
+      <c r="B83" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="10"/>
-      <c r="B84" s="10"/>
-    </row>
-    <row r="85" ht="24.75" spans="1:2">
-      <c r="A85" s="3" t="s">
+    <row r="84" ht="15" spans="1:2">
+      <c r="A84" s="4"/>
+      <c r="B84" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" ht="30" spans="1:3">
+      <c r="A85" s="4"/>
+      <c r="B85" t="s">
         <v>97</v>
       </c>
-      <c r="B85" s="3"/>
-    </row>
-    <row r="86" ht="15" spans="1:2">
-      <c r="A86" s="4" t="s">
+      <c r="C85" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="4"/>
+      <c r="B86" t="s">
         <v>98</v>
       </c>
-      <c r="B86" s="11" t="s">
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="4"/>
+      <c r="B87" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="87" ht="15" spans="1:2">
-      <c r="A87" s="4"/>
-      <c r="B87" s="11" t="s">
+    <row r="88" ht="18" spans="1:2">
+      <c r="A88" s="4"/>
+      <c r="B88" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="89" ht="18" spans="1:2">
+      <c r="A89" s="4"/>
+      <c r="B89" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="88" ht="15" spans="1:2">
-      <c r="A88" s="4"/>
-      <c r="B88" s="11" t="s">
+    <row r="90" ht="18" spans="1:2">
+      <c r="A90" s="4"/>
+      <c r="B90" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="89" ht="15" spans="1:2">
-      <c r="A89" s="4"/>
-      <c r="B89" s="11" t="s">
+    <row r="91" ht="18" spans="1:2">
+      <c r="A91" s="4"/>
+      <c r="B91" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="90" ht="15" spans="1:2">
-      <c r="A90" s="4"/>
-      <c r="B90" s="11" t="s">
+    <row r="92" ht="18" spans="1:2">
+      <c r="A92" s="4"/>
+      <c r="B92" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="91" ht="15" spans="1:2">
-      <c r="A91" s="4"/>
-      <c r="B91" s="11" t="s">
+    <row r="93" ht="18" spans="1:2">
+      <c r="A93" s="4"/>
+      <c r="B93" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="92" ht="15" spans="1:2">
-      <c r="A92" s="4"/>
-      <c r="B92" s="11" t="s">
+    <row r="94" ht="18" spans="1:2">
+      <c r="A94" s="4"/>
+      <c r="B94" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="93" ht="15" spans="1:2">
-      <c r="A93" s="4"/>
-      <c r="B93" s="11" t="s">
+    <row r="95" spans="1:2">
+      <c r="A95" s="10"/>
+      <c r="B95" s="10"/>
+    </row>
+    <row r="96" ht="24.75" spans="1:2">
+      <c r="A96" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="94" ht="15" spans="1:2">
-      <c r="A94" s="4"/>
-      <c r="B94" s="11" t="s">
+      <c r="B96" s="3"/>
+    </row>
+    <row r="97" ht="15" spans="1:2">
+      <c r="A97" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="95" ht="15" spans="1:2">
-      <c r="A95" s="4"/>
-      <c r="B95" s="11" t="s">
+      <c r="B97" s="11" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="96" ht="15" spans="1:2">
-      <c r="A96" s="4"/>
-      <c r="B96" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="97" ht="15" spans="1:2">
-      <c r="A97" s="4"/>
-      <c r="B97" s="11" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="98" ht="15" spans="1:2">
       <c r="A98" s="4"/>
-      <c r="B98" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="99" ht="30" spans="1:3">
+      <c r="B98" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="99" ht="15" spans="1:2">
       <c r="A99" s="4"/>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="100" ht="15" spans="1:2">
+      <c r="A100" s="4"/>
+      <c r="B100" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C99" s="21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="100" ht="15" spans="1:5">
-      <c r="A100" s="4"/>
-      <c r="B100" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E100" s="14"/>
     </row>
     <row r="101" ht="15" spans="1:2">
       <c r="A101" s="4"/>
-      <c r="B101" s="6" t="s">
-        <v>30</v>
+      <c r="B101" s="11" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="102" ht="15" spans="1:2">
       <c r="A102" s="4"/>
-      <c r="B102" s="5" t="s">
-        <v>114</v>
+      <c r="B102" s="11" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="103" ht="15" spans="1:2">
       <c r="A103" s="4"/>
-      <c r="B103" s="5" t="s">
-        <v>115</v>
+      <c r="B103" s="11" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="104" ht="15" spans="1:2">
       <c r="A104" s="4"/>
-      <c r="B104" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="105" ht="30" spans="1:3">
+      <c r="B104" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="105" ht="15" spans="1:2">
       <c r="A105" s="4"/>
-      <c r="B105" s="5" t="s">
+      <c r="B105" s="11" t="s">
         <v>116</v>
-      </c>
-      <c r="C105" s="21" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="106" ht="15" spans="1:2">
       <c r="A106" s="4"/>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="11" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="107" ht="15" spans="1:2">
       <c r="A107" s="4"/>
-      <c r="B107" s="5" t="s">
+      <c r="B107" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="108" ht="9" customHeight="1" spans="1:2">
-      <c r="A108" s="10"/>
-      <c r="B108" s="10"/>
-    </row>
-    <row r="109" s="1" customFormat="1" ht="24.75" spans="1:2">
-      <c r="A109" s="3" t="s">
+    <row r="108" ht="15" spans="1:2">
+      <c r="A108" s="4"/>
+      <c r="B108" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B109" s="3"/>
-    </row>
-    <row r="110" s="1" customFormat="1" ht="15" spans="1:2">
-      <c r="A110" s="4" t="s">
+    </row>
+    <row r="109" ht="15" spans="1:2">
+      <c r="A109" s="4"/>
+      <c r="B109" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="110" ht="30" spans="1:3">
+      <c r="A110" s="4"/>
+      <c r="B110" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B110" s="11" t="s">
+      <c r="C110" s="19" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="111" s="1" customFormat="1" ht="23" customHeight="1" spans="1:2">
+    <row r="111" ht="15" spans="1:5">
       <c r="A111" s="4"/>
-      <c r="B111" s="11" t="s">
+      <c r="B111" s="5" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="112" s="1" customFormat="1" ht="15" spans="1:2">
+      <c r="E111" s="14"/>
+    </row>
+    <row r="112" ht="15" spans="1:2">
       <c r="A112" s="4"/>
-      <c r="B112" s="11" t="s">
+      <c r="B112" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="113" ht="15" spans="1:2">
+      <c r="A113" s="4"/>
+      <c r="B113" s="5" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="113" s="1" customFormat="1" ht="15" spans="1:2">
-      <c r="A113" s="4"/>
-      <c r="B113" s="11" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="114" ht="15" spans="1:2">
       <c r="A114" s="4"/>
-      <c r="B114" s="11" t="s">
+      <c r="B114" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="115" ht="15" spans="1:2">
+      <c r="A115" s="4"/>
+      <c r="B115" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="116" ht="30" spans="1:3">
+      <c r="A116" s="4"/>
+      <c r="B116" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="115" spans="1:2">
-      <c r="A115" s="4"/>
-      <c r="B115" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="116" ht="15" spans="1:2">
-      <c r="A116" s="4"/>
-      <c r="B116" s="11" t="s">
-        <v>127</v>
+      <c r="C116" s="19" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="117" ht="15" spans="1:2">
       <c r="A117" s="4"/>
-      <c r="B117" s="11" t="s">
-        <v>128</v>
+      <c r="B117" s="5" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="118" ht="15" spans="1:2">
       <c r="A118" s="4"/>
-      <c r="B118" s="11" t="s">
+      <c r="B118" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="119" ht="9" customHeight="1" spans="1:2">
+      <c r="A119" s="10"/>
+      <c r="B119" s="10"/>
+    </row>
+    <row r="120" s="1" customFormat="1" ht="24.75" spans="1:2">
+      <c r="A120" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B120" s="3"/>
+    </row>
+    <row r="121" s="1" customFormat="1" ht="15" spans="1:2">
+      <c r="A121" s="4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="119" ht="15" spans="1:2">
-      <c r="A119" s="4"/>
-      <c r="B119" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="120" ht="30" spans="1:3">
-      <c r="A120" s="4"/>
-      <c r="B120" s="11" t="s">
+      <c r="B121" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C120" s="7" t="s">
+    </row>
+    <row r="122" s="1" customFormat="1" ht="23" customHeight="1" spans="1:2">
+      <c r="A122" s="4"/>
+      <c r="B122" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="121" ht="15" spans="1:2">
-      <c r="A121" s="4"/>
-      <c r="B121" s="11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="122" ht="15" spans="1:2">
-      <c r="A122" s="4"/>
-      <c r="B122" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="123" ht="30" spans="1:2">
+    <row r="123" s="1" customFormat="1" ht="15" spans="1:2">
       <c r="A123" s="4"/>
       <c r="B123" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="124" s="1" customFormat="1" ht="15" spans="1:2">
+      <c r="A124" s="4"/>
+      <c r="B124" s="11" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="124" ht="15" spans="1:2">
-      <c r="A124" s="4"/>
-      <c r="B124" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="125" ht="30" spans="1:3">
+    <row r="125" ht="15" spans="1:2">
       <c r="A125" s="4"/>
       <c r="B125" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="C125" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="126" ht="15" spans="1:2">
+    </row>
+    <row r="126" spans="1:2">
       <c r="A126" s="4"/>
-      <c r="B126" s="11" t="s">
+      <c r="B126" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2828,40 +2857,130 @@
         <v>136</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
-      <c r="A128" s="10"/>
-      <c r="B128" s="10"/>
+    <row r="128" ht="15" spans="1:2">
+      <c r="A128" s="4"/>
+      <c r="B128" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="129" ht="15" spans="1:2">
+      <c r="A129" s="4"/>
+      <c r="B129" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="130" ht="15" spans="1:2">
+      <c r="A130" s="4"/>
+      <c r="B130" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="131" ht="30" spans="1:3">
+      <c r="A131" s="4"/>
+      <c r="B131" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C131" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="132" ht="15" spans="1:2">
+      <c r="A132" s="4"/>
+      <c r="B132" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="133" ht="15" spans="1:2">
+      <c r="A133" s="4"/>
+      <c r="B133" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="134" ht="30" spans="1:2">
+      <c r="A134" s="4"/>
+      <c r="B134" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="135" ht="15" spans="1:2">
+      <c r="A135" s="4"/>
+      <c r="B135" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="136" ht="30" spans="1:3">
+      <c r="A136" s="4"/>
+      <c r="B136" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="137" ht="15" spans="1:2">
+      <c r="A137" s="4"/>
+      <c r="B137" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="138" ht="15" spans="1:2">
+      <c r="A138" s="4"/>
+      <c r="B138" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="139" ht="18" spans="1:2">
+      <c r="A139" s="4"/>
+      <c r="B139" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="140" ht="18" spans="1:2">
+      <c r="A140" s="4"/>
+      <c r="B140" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="141" ht="18" spans="1:2">
+      <c r="A141" s="4"/>
+      <c r="B141" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="10"/>
+      <c r="B142" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A120:B120"/>
     <mergeCell ref="A3:A24"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="A36:A55"/>
-    <mergeCell ref="A58:A83"/>
-    <mergeCell ref="A86:A107"/>
-    <mergeCell ref="A110:A127"/>
+    <mergeCell ref="A29:A36"/>
+    <mergeCell ref="A38:A57"/>
+    <mergeCell ref="A62:A87"/>
+    <mergeCell ref="A97:A118"/>
+    <mergeCell ref="A121:A138"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="2. Module Outline"/>
-    <hyperlink ref="B31" r:id="rId2" display="16. New Patterns: The Predicate Interface Example"/>
+    <hyperlink ref="B33" r:id="rId2" display="16. New Patterns: The Predicate Interface Example"/>
     <hyperlink ref="C15" r:id="rId3" display="https://www.hackerrank.com/challenges/java-lambda-expressions/problem" tooltip="https://www.hackerrank.com/challenges/java-lambda-expressions/problem"/>
     <hyperlink ref="C16" r:id="rId4" display="https://www.hackerrank.com/challenges/dynamic-array/problem" tooltip="https://www.hackerrank.com/challenges/dynamic-array/problem"/>
     <hyperlink ref="C23" r:id="rId5" display="https://www.hackerrank.com/challenges/array-left-rotation" tooltip="https://www.hackerrank.com/challenges/array-left-rotation"/>
     <hyperlink ref="C22" r:id="rId6" display="https://www.hackerrank.com/challenges/sparse-arrays/problem" tooltip="https://www.hackerrank.com/challenges/sparse-arrays/problem"/>
     <hyperlink ref="C24" r:id="rId7" display="https://www.hackerrank.com/challenges/java-loops-i/problem"/>
-    <hyperlink ref="C48" r:id="rId8" display="https://www.hackerrank.com/interview/interview-preparation-kit/arrays/challenges"/>
-    <hyperlink ref="C54" r:id="rId8" display="https://www.hackerrank.com/interview/interview-preparation-kit/arrays/challenges"/>
-    <hyperlink ref="C75" r:id="rId9" display="https://www.hackerrank.com/interview/interview-preparation-kit/dictionaries-hashmaps/challenges"/>
-    <hyperlink ref="C81" r:id="rId9" display="https://www.hackerrank.com/interview/interview-preparation-kit/dictionaries-hashmaps/challenges"/>
-    <hyperlink ref="C99" r:id="rId10" display="https://www.hackerrank.com/interview/interview-preparation-kit/sorting/challenges"/>
-    <hyperlink ref="C105" r:id="rId10" display="https://www.hackerrank.com/interview/interview-preparation-kit/sorting/challenges"/>
-    <hyperlink ref="C120" r:id="rId11" display="https://www.hackerrank.com/interview/interview-preparation-kit/strings/challenges"/>
-    <hyperlink ref="C125" r:id="rId11" display="https://www.hackerrank.com/interview/interview-preparation-kit/strings/challenges"/>
+    <hyperlink ref="C50" r:id="rId8" display="https://www.hackerrank.com/interview/interview-preparation-kit/arrays/challenges"/>
+    <hyperlink ref="C56" r:id="rId8" display="https://www.hackerrank.com/interview/interview-preparation-kit/arrays/challenges"/>
+    <hyperlink ref="C79" r:id="rId9" display="https://www.hackerrank.com/interview/interview-preparation-kit/dictionaries-hashmaps/challenges"/>
+    <hyperlink ref="C85" r:id="rId9" display="https://www.hackerrank.com/interview/interview-preparation-kit/dictionaries-hashmaps/challenges"/>
+    <hyperlink ref="C110" r:id="rId10" display="https://www.hackerrank.com/interview/interview-preparation-kit/sorting/challenges"/>
+    <hyperlink ref="C116" r:id="rId10" display="https://www.hackerrank.com/interview/interview-preparation-kit/sorting/challenges"/>
+    <hyperlink ref="C131" r:id="rId11" display="https://www.hackerrank.com/interview/interview-preparation-kit/strings/challenges"/>
+    <hyperlink ref="C136" r:id="rId11" display="https://www.hackerrank.com/interview/interview-preparation-kit/strings/challenges"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -2899,172 +3018,172 @@
     </row>
     <row r="2" ht="27" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" ht="27" customHeight="1" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" ht="27" customHeight="1" spans="1:2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" ht="27" customHeight="1" spans="1:2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" ht="27" customHeight="1" spans="1:2">
       <c r="A6" s="4"/>
       <c r="B6" s="5" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" ht="27" customHeight="1" spans="1:2">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" ht="27" customHeight="1" spans="1:2">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" ht="27" customHeight="1" spans="1:2">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" ht="12" customHeight="1"/>
     <row r="11" ht="15" spans="1:2">
       <c r="A11" s="4" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:2">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:2">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:2">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:2">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:2">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:2">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="4"/>
       <c r="B19" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:2">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" customFormat="1" ht="15" spans="1:3">
       <c r="A21" s="4"/>
       <c r="B21" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C21" s="7"/>
     </row>
     <row r="22" customFormat="1" ht="30" spans="1:3">
       <c r="A22" s="4"/>
       <c r="B22" s="8" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" customFormat="1" ht="15" spans="1:3">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="C23" s="7"/>
     </row>
     <row r="24" customFormat="1" ht="15" spans="1:3">
       <c r="A24" s="4"/>
       <c r="B24" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C24" s="7"/>
     </row>
     <row r="25" customFormat="1" ht="30" spans="1:3">
       <c r="A25" s="4"/>
       <c r="B25" s="8" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" customFormat="1" spans="1:2">
       <c r="A26" s="4"/>
       <c r="B26" s="8" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" customFormat="1" spans="1:2">
       <c r="A27" s="4"/>
       <c r="B27" s="8" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" customFormat="1" spans="1:2">
       <c r="A28" s="4"/>
       <c r="B28" s="8" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:2">
@@ -3073,70 +3192,70 @@
     </row>
     <row r="30" ht="24.75" spans="1:2">
       <c r="A30" s="3" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="B30" s="3"/>
     </row>
     <row r="31" customFormat="1" ht="15" spans="1:2">
       <c r="A31" s="4" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" customFormat="1" ht="15" spans="1:2">
       <c r="A32" s="4"/>
       <c r="B32" s="5" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" customFormat="1" ht="15" spans="1:2">
       <c r="A33" s="4"/>
       <c r="B33" s="5" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" customFormat="1" ht="15" spans="1:2">
       <c r="A34" s="4"/>
       <c r="B34" s="5" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" customFormat="1" ht="15" spans="1:2">
       <c r="A35" s="4"/>
       <c r="B35" s="5" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" customFormat="1" ht="15" spans="1:2">
       <c r="A36" s="4"/>
       <c r="B36" s="11" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" customFormat="1" ht="15" spans="1:2">
       <c r="A37" s="4"/>
       <c r="B37" s="11" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" customFormat="1" ht="15" spans="1:2">
       <c r="A38" s="4"/>
       <c r="B38" s="11" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" customFormat="1" ht="15" spans="1:2">
       <c r="A39" s="4"/>
       <c r="B39" s="5" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" customFormat="1" ht="15" spans="1:2">
       <c r="A40" s="4"/>
       <c r="B40" s="5" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" customFormat="1" spans="1:1">
@@ -3145,88 +3264,88 @@
     <row r="42" ht="11" customHeight="1"/>
     <row r="43" customFormat="1" ht="15" spans="1:2">
       <c r="A43" s="4" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" customFormat="1" ht="15" spans="1:2">
       <c r="A44" s="4"/>
       <c r="B44" s="5" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
     </row>
     <row r="45" customFormat="1" ht="15" spans="1:2">
       <c r="A45" s="4"/>
       <c r="B45" s="5" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" customFormat="1" ht="15" spans="1:2">
       <c r="A46" s="4"/>
       <c r="B46" s="5" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" customFormat="1" ht="15" spans="1:2">
       <c r="A47" s="4"/>
       <c r="B47" s="5" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
     </row>
     <row r="48" customFormat="1" ht="15" spans="1:2">
       <c r="A48" s="4"/>
       <c r="B48" s="5" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" customFormat="1" ht="15" spans="1:2">
       <c r="A49" s="4"/>
       <c r="B49" s="5" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:2">
       <c r="A50" s="4"/>
       <c r="B50" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" ht="30" spans="1:3">
       <c r="A51" s="4"/>
       <c r="B51" s="12" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:2">
       <c r="A52" s="4"/>
       <c r="B52" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" ht="30" spans="1:3">
       <c r="A53" s="4"/>
       <c r="B53" s="12" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="4"/>
       <c r="B54" s="12" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="4"/>
       <c r="B55" s="12" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -3235,156 +3354,156 @@
     </row>
     <row r="57" ht="24.75" spans="1:2">
       <c r="A57" s="3" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="B57" s="3"/>
     </row>
     <row r="58" ht="15" spans="1:2">
       <c r="A58" s="4" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="4"/>
       <c r="B59" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="4"/>
       <c r="B60" s="13" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
     </row>
     <row r="61" ht="15" spans="1:2">
       <c r="A61" s="4"/>
       <c r="B61" s="11" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
     </row>
     <row r="62" ht="15" spans="1:2">
       <c r="A62" s="4"/>
       <c r="B62" s="5" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63" ht="15" spans="1:2">
       <c r="A63" s="4"/>
       <c r="B63" s="5" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
     </row>
     <row r="64" ht="15" spans="1:2">
       <c r="A64" s="4"/>
       <c r="B64" s="5" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="4" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="B66" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="4"/>
       <c r="B67" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="4"/>
       <c r="B68" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="4"/>
       <c r="B69" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="4"/>
       <c r="B70" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="4"/>
       <c r="B71" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="4"/>
       <c r="B72" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="4"/>
       <c r="B73" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
     </row>
     <row r="74" ht="18" spans="1:2">
       <c r="A74" s="4"/>
       <c r="B74" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="75" ht="30" spans="1:3">
       <c r="A75" s="4"/>
       <c r="B75" s="12" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
     </row>
     <row r="76" ht="18" spans="1:2">
       <c r="A76" s="4"/>
       <c r="B76" s="12" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
     </row>
     <row r="77" ht="18" spans="1:2">
       <c r="A77" s="4"/>
       <c r="B77" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="78" ht="30" spans="1:3">
       <c r="A78" s="4"/>
       <c r="B78" s="12" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
     </row>
     <row r="79" ht="18" spans="1:2">
       <c r="A79" s="4"/>
       <c r="B79" s="12" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
     </row>
     <row r="80" ht="18" spans="1:2">
       <c r="A80" s="4"/>
       <c r="B80" s="12" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
     </row>
     <row r="81" ht="18" spans="1:2">
       <c r="A81" s="4"/>
       <c r="B81" s="12" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -3393,40 +3512,40 @@
     </row>
     <row r="83" ht="24.75" spans="1:2">
       <c r="A83" s="3" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="B83" s="3"/>
     </row>
     <row r="84" ht="15" spans="1:2">
       <c r="A84" s="4" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
     </row>
     <row r="85" ht="15" spans="1:2">
       <c r="A85" s="4"/>
       <c r="B85" s="11" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
     </row>
     <row r="86" ht="15" spans="1:2">
       <c r="A86" s="4"/>
       <c r="B86" s="11" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
     </row>
     <row r="87" ht="15" spans="1:2">
       <c r="A87" s="4"/>
       <c r="B87" s="11" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
     </row>
     <row r="88" ht="15" spans="1:2">
       <c r="A88" s="4"/>
       <c r="B88" s="11" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
     </row>
     <row r="89" ht="18" spans="1:1">
@@ -3434,77 +3553,77 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="4" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="B90" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="4"/>
       <c r="B91" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="E91" s="14"/>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="4"/>
       <c r="B92" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="4"/>
       <c r="B93" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
     </row>
     <row r="94" ht="18" spans="1:2">
       <c r="A94" s="4"/>
       <c r="B94" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="95" ht="30" spans="1:3">
       <c r="A95" s="4"/>
       <c r="B95" s="12" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
     </row>
     <row r="96" ht="18" spans="1:2">
       <c r="A96" s="4"/>
       <c r="B96" s="12" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
     </row>
     <row r="97" ht="18" spans="1:2">
       <c r="A97" s="4"/>
       <c r="B97" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="98" ht="30" spans="1:3">
       <c r="A98" s="4"/>
       <c r="B98" s="12" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
     </row>
     <row r="99" ht="18" spans="1:2">
       <c r="A99" s="4"/>
       <c r="B99" s="12" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
     </row>
     <row r="100" ht="18" spans="1:2">
       <c r="A100" s="4"/>
       <c r="B100" s="12" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
     </row>
     <row r="101" ht="9" customHeight="1" spans="1:2">
@@ -3513,130 +3632,130 @@
     </row>
     <row r="102" s="1" customFormat="1" ht="24.75" spans="1:2">
       <c r="A102" s="3" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="B102" s="3"/>
     </row>
     <row r="103" s="1" customFormat="1" ht="15" spans="1:2">
       <c r="A103" s="4" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
     </row>
     <row r="104" s="1" customFormat="1" ht="18" customHeight="1" spans="1:2">
       <c r="A104" s="4"/>
       <c r="B104" s="11" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
     </row>
     <row r="105" s="1" customFormat="1" ht="15" spans="1:2">
       <c r="A105" s="4"/>
       <c r="B105" s="11" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
     </row>
     <row r="106" s="1" customFormat="1" ht="15" spans="1:2">
       <c r="A106" s="4"/>
       <c r="B106" s="11" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
     </row>
     <row r="107" ht="15" spans="1:2">
       <c r="A107" s="4"/>
       <c r="B107" s="11" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="4"/>
       <c r="B108" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
     </row>
     <row r="109" ht="18" spans="1:2">
       <c r="A109" s="4"/>
       <c r="B109" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="110" ht="30" spans="1:3">
       <c r="A110" s="4"/>
       <c r="B110" s="12" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
     </row>
     <row r="111" ht="18" spans="1:2">
       <c r="A111" s="4"/>
       <c r="B111" s="12" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
     </row>
     <row r="112" ht="30" spans="1:3">
       <c r="A112" s="4"/>
       <c r="B112" s="12" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
     </row>
     <row r="113" ht="18" spans="1:2">
       <c r="A113" s="4"/>
       <c r="B113" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="114" ht="30" spans="1:3">
       <c r="A114" s="4"/>
       <c r="B114" s="12" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
     </row>
     <row r="115" ht="18" spans="1:2">
       <c r="A115" s="4"/>
       <c r="B115" s="12" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
     </row>
     <row r="116" ht="18" spans="1:2">
       <c r="A116" s="4"/>
       <c r="B116" s="12" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
     </row>
     <row r="117" ht="30" spans="1:3">
       <c r="A117" s="4"/>
       <c r="B117" s="12" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
     </row>
     <row r="118" ht="18" spans="1:2">
       <c r="A118" s="4"/>
       <c r="B118" s="12" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
     </row>
     <row r="119" ht="18" spans="1:2">
       <c r="A119" s="4"/>
       <c r="B119" s="12" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
     </row>
     <row r="120" ht="18" spans="1:2">
       <c r="A120" s="4"/>
       <c r="B120" s="12" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
     </row>
     <row r="121" spans="1:2">

</xml_diff>

<commit_message>
Added Course Materials - Day5 .
</commit_message>
<xml_diff>
--- a/Java 8 & 11 - TOC.xlsx
+++ b/Java 8 & 11 - TOC.xlsx
@@ -800,9 +800,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="29">
@@ -892,29 +892,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -922,21 +900,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -950,7 +913,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1011,6 +974,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1046,7 +1046,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1058,121 +1172,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1190,43 +1190,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1307,30 +1307,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1394,6 +1370,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1407,15 +1407,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1428,131 +1428,131 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1599,6 +1599,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1968,56 +1971,56 @@
   <sheetData>
     <row r="7" ht="13.5"/>
     <row r="8" ht="13.5" spans="6:9">
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="22" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="6:9">
-      <c r="F9" s="22">
+      <c r="F9" s="23">
         <v>1</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="25">
         <v>5</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="25">
         <v>20</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="6:9">
-      <c r="F10" s="25">
+      <c r="F10" s="26">
         <v>2</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="G10" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="25">
         <v>5</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="25">
         <v>20</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="6:9">
-      <c r="F11" s="27"/>
-      <c r="G11" s="28" t="s">
+      <c r="F11" s="28"/>
+      <c r="G11" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="I11" s="30" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2033,9 +2036,9 @@
   <dimension ref="A1:E142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
+      <selection pane="bottomLeft" activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -2552,7 +2555,7 @@
     </row>
     <row r="79" ht="30" spans="1:3">
       <c r="A79" s="4"/>
-      <c r="B79" t="s">
+      <c r="B79" s="10" t="s">
         <v>92</v>
       </c>
       <c r="C79" s="9" t="s">
@@ -2561,7 +2564,7 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="4"/>
-      <c r="B80" t="s">
+      <c r="B80" s="10" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2787,7 +2790,7 @@
       <c r="B116" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C116" s="19" t="s">
+      <c r="C116" s="20" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Training Materials - Day 6.
</commit_message>
<xml_diff>
--- a/Java 8 & 11 - TOC.xlsx
+++ b/Java 8 & 11 - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="226">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -456,90 +456,66 @@
     <t>Common Child</t>
   </si>
   <si>
+    <t>Counting Bits</t>
+  </si>
+  <si>
+    <t>Skip A Level</t>
+  </si>
+  <si>
+    <t>Day 6</t>
+  </si>
+  <si>
+    <t>1. Introducing Java 11</t>
+  </si>
+  <si>
+    <t>1. Course Overview</t>
+  </si>
+  <si>
+    <t>2. Java 11 Introduction</t>
+  </si>
+  <si>
+    <t>3. Oracle JDK &amp; OpenJDK</t>
+  </si>
+  <si>
+    <t>4. Long-Term-Support</t>
+  </si>
+  <si>
+    <t>5. Launching Single-file Source Code</t>
+  </si>
+  <si>
+    <t>6. Demo: Launching Single-file Source Code</t>
+  </si>
+  <si>
+    <t>10. Summary</t>
+  </si>
+  <si>
+    <t>Hash Tables: Ice Cream Parlor</t>
+  </si>
+  <si>
+    <t>https://www.hackerrank.com/interview/interview-preparation-kit/search/challenges</t>
+  </si>
+  <si>
+    <t>Swap Nodes [Algo]</t>
+  </si>
+  <si>
+    <t>Pairs</t>
+  </si>
+  <si>
+    <t>Triple sum</t>
+  </si>
+  <si>
+    <t>Minimum Time Required</t>
+  </si>
+  <si>
+    <t>Maximum Subarray Sum</t>
+  </si>
+  <si>
     <t>Aladdin and his Carpet</t>
   </si>
   <si>
     <t>Slot Machine 2.0</t>
   </si>
   <si>
-    <t>Day 6</t>
-  </si>
-  <si>
-    <t>1. Introducing Java 11</t>
-  </si>
-  <si>
-    <t>1. Course Overview</t>
-  </si>
-  <si>
-    <t>2. Java 11 Introduction</t>
-  </si>
-  <si>
-    <t>3. Oracle JDK &amp; OpenJDK</t>
-  </si>
-  <si>
-    <t>4. Long-Term-Support</t>
-  </si>
-  <si>
-    <t>5. Launching Single-file Source Code</t>
-  </si>
-  <si>
-    <t>6. Demo: Launching Single-file Source Code</t>
-  </si>
-  <si>
-    <t>10. Summary</t>
-  </si>
-  <si>
-    <t>2. Working with Lambda Expressions in Oracle Java SE 11</t>
-  </si>
-  <si>
-    <t>1.  Overview</t>
-  </si>
-  <si>
-    <t>2. Introduction</t>
-  </si>
-  <si>
-    <t>3. Lambda Expressions - First Look</t>
-  </si>
-  <si>
-    <t>4. Functional Interfaces - First Look</t>
-  </si>
-  <si>
-    <t>5. Syntax of Lambda Expressions</t>
-  </si>
-  <si>
-    <t>6. Capturing Variables in Lambda Expressions</t>
-  </si>
-  <si>
-    <t>7. Interaction of Lambda Expressions with Enclosing Code</t>
-  </si>
-  <si>
-    <t>8. Working with Exceptions in Lambda Expressions</t>
-  </si>
-  <si>
-    <t>9. Method References</t>
-  </si>
-  <si>
-    <t>Hash Tables: Ice Cream Parlor</t>
-  </si>
-  <si>
-    <t>https://www.hackerrank.com/interview/interview-preparation-kit/search/challenges</t>
-  </si>
-  <si>
-    <t>Swap Nodes [Algo]</t>
-  </si>
-  <si>
-    <t>Pairs</t>
-  </si>
-  <si>
-    <t>Triple sum</t>
-  </si>
-  <si>
-    <t>Minimum Time Required</t>
-  </si>
-  <si>
-    <t>Maximum Subarray Sum</t>
-  </si>
-  <si>
     <t>Day 7</t>
   </si>
   <si>
@@ -576,93 +552,48 @@
     <t>10.Summary</t>
   </si>
   <si>
-    <t xml:space="preserve">4. Working with Functional Interfaces </t>
-  </si>
-  <si>
-    <t>1. Overview</t>
-  </si>
-  <si>
-    <t>2. Understanding Functional Interfaces</t>
-  </si>
-  <si>
-    <t>3. Common Standard Functional Interfaces</t>
-  </si>
-  <si>
-    <t>4. Practical Examples of Standard Functional Interfaces</t>
-  </si>
-  <si>
-    <t>5. Functional Composition</t>
-  </si>
-  <si>
-    <t>6. Specialized Standard Functional Interfaces</t>
+    <t>Max Array Sum</t>
+  </si>
+  <si>
+    <t>https://www.hackerrank.com/interview/interview-preparation-kit/dynamic-programming/challenges</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>Candies</t>
+  </si>
+  <si>
+    <t>Decibinary Numbers</t>
+  </si>
+  <si>
+    <t>Day 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.  Performance and Security Improvements </t>
+  </si>
+  <si>
+    <t>1. Garbage Collection Improvements</t>
+  </si>
+  <si>
+    <t>2. Epsilon: A No-Op Garbage Collector</t>
+  </si>
+  <si>
+    <t>3. Improved Aarch64 Intrinsics</t>
+  </si>
+  <si>
+    <t>4.  Flight Recorder</t>
+  </si>
+  <si>
+    <t>5.  Dynamic Class-File Constants</t>
+  </si>
+  <si>
+    <t>6. Security Improvement: TLS 1.3</t>
   </si>
   <si>
     <t>7. Summary</t>
   </si>
   <si>
-    <t>Max Array Sum</t>
-  </si>
-  <si>
-    <t>https://www.hackerrank.com/interview/interview-preparation-kit/dynamic-programming/challenges</t>
-  </si>
-  <si>
-    <t>Abbreviation</t>
-  </si>
-  <si>
-    <t>Candies</t>
-  </si>
-  <si>
-    <t>Decibinary Numbers</t>
-  </si>
-  <si>
-    <t>Day 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.  Performance and Security Improvements </t>
-  </si>
-  <si>
-    <t>1. Garbage Collection Improvements</t>
-  </si>
-  <si>
-    <t>2. Epsilon: A No-Op Garbage Collector</t>
-  </si>
-  <si>
-    <t>3. Improved Aarch64 Intrinsics</t>
-  </si>
-  <si>
-    <t>4.  Flight Recorder</t>
-  </si>
-  <si>
-    <t>5.  Dynamic Class-File Constants</t>
-  </si>
-  <si>
-    <t>6. Security Improvement: TLS 1.3</t>
-  </si>
-  <si>
-    <t>6. Working with Streams - The Basics</t>
-  </si>
-  <si>
-    <t>2. Understanding Streams</t>
-  </si>
-  <si>
-    <t>3. Differences between Streams and Collections</t>
-  </si>
-  <si>
-    <t>4. Obtaining Streams</t>
-  </si>
-  <si>
-    <t>5. Filtering and Transforming Streams</t>
-  </si>
-  <si>
-    <t>6. Searching in Streams</t>
-  </si>
-  <si>
-    <t>7. Reducing and Collecting Streams</t>
-  </si>
-  <si>
-    <t>8. Summary</t>
-  </si>
-  <si>
     <t>Balanced Brackets</t>
   </si>
   <si>
@@ -705,18 +636,6 @@
     <t>5. Summary</t>
   </si>
   <si>
-    <t>8. Working with Streams - In Depth</t>
-  </si>
-  <si>
-    <t>2. Generating and Building Streams</t>
-  </si>
-  <si>
-    <t>3. Reducing Streams in Detail</t>
-  </si>
-  <si>
-    <t>4. Collecting Streams in Detail</t>
-  </si>
-  <si>
     <t>Roads and Libraries</t>
   </si>
   <si>
@@ -738,25 +657,7 @@
     <t>Day 10</t>
   </si>
   <si>
-    <t>9. Working with Streams - In Depth</t>
-  </si>
-  <si>
-    <t>5. Working with Collectors</t>
-  </si>
-  <si>
-    <t>6. Grouping Stream Elements</t>
-  </si>
-  <si>
-    <t>7. Partitioning Stream Elements</t>
-  </si>
-  <si>
-    <t>8. Parallel Streams</t>
-  </si>
-  <si>
-    <t>9. Specialized Streams</t>
-  </si>
-  <si>
-    <t>10. Course Summary</t>
+    <t>Hands On Demos</t>
   </si>
   <si>
     <t>Tree: Height of a Binary Tree</t>
@@ -800,10 +701,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -865,16 +766,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10.5"/>
+      <color rgb="FFB7C9CC"/>
+      <name val="var(--font-family-text)"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="9.95"/>
       <color rgb="FF0000FF"/>
       <name val="NimbusRomNo9L-Medi"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color rgb="FFB7C9CC"/>
-      <name val="var(--font-family-text)"/>
       <charset val="134"/>
     </font>
     <font>
@@ -892,14 +793,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -921,9 +823,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -943,10 +845,34 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -966,11 +892,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -981,24 +906,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1006,14 +915,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1046,7 +947,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1058,25 +965,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1094,7 +983,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1106,13 +1031,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1124,67 +1103,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1196,37 +1121,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1307,21 +1208,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1363,9 +1249,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1388,34 +1291,32 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1428,131 +1329,131 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1587,7 +1488,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1597,12 +1497,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1971,56 +1873,56 @@
   <sheetData>
     <row r="7" ht="13.5"/>
     <row r="8" ht="13.5" spans="6:9">
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="23" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="6:9">
-      <c r="F9" s="23">
+      <c r="F9" s="24">
         <v>1</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="26">
         <v>5</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="26">
         <v>20</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="6:9">
-      <c r="F10" s="26">
+      <c r="F10" s="27">
         <v>2</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="26">
         <v>5</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="26">
         <v>20</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="6:9">
-      <c r="F11" s="28"/>
-      <c r="G11" s="29" t="s">
+      <c r="F11" s="29"/>
+      <c r="G11" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="31" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2035,10 +1937,10 @@
   <sheetPr/>
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C110" sqref="C110"/>
+      <selection pane="bottomLeft" activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -2135,13 +2037,13 @@
     </row>
     <row r="14" customFormat="1" ht="15" spans="1:2">
       <c r="A14" s="4"/>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="1" ht="30" spans="1:3">
       <c r="A15" s="4"/>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -2150,7 +2052,7 @@
     </row>
     <row r="16" customFormat="1" ht="30" spans="1:3">
       <c r="A16" s="4"/>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -2189,7 +2091,7 @@
     </row>
     <row r="22" customFormat="1" ht="30" spans="1:3">
       <c r="A22" s="4"/>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -2198,7 +2100,7 @@
     </row>
     <row r="23" customFormat="1" ht="30" spans="1:3">
       <c r="A23" s="4"/>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -2207,7 +2109,7 @@
     </row>
     <row r="24" customFormat="1" ht="30" spans="1:3">
       <c r="A24" s="4"/>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="16" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -2263,7 +2165,7 @@
       <c r="B32" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="18"/>
+      <c r="C32" s="17"/>
     </row>
     <row r="33" customFormat="1" ht="15" spans="1:2">
       <c r="A33" s="4"/>
@@ -2747,7 +2649,7 @@
     </row>
     <row r="110" ht="30" spans="1:3">
       <c r="A110" s="4"/>
-      <c r="B110" s="5" t="s">
+      <c r="B110" s="18" t="s">
         <v>120</v>
       </c>
       <c r="C110" s="19" t="s">
@@ -2756,10 +2658,10 @@
     </row>
     <row r="111" ht="15" spans="1:5">
       <c r="A111" s="4"/>
-      <c r="B111" s="5" t="s">
+      <c r="B111" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="E111" s="14"/>
+      <c r="E111" s="20"/>
     </row>
     <row r="112" ht="15" spans="1:2">
       <c r="A112" s="4"/>
@@ -2790,7 +2692,7 @@
       <c r="B116" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C116" s="20" t="s">
+      <c r="C116" s="21" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2993,15 +2895,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="35.125" customWidth="1"/>
     <col min="2" max="2" width="43.75" customWidth="1"/>
@@ -3070,731 +2972,527 @@
       </c>
     </row>
     <row r="10" ht="12" customHeight="1"/>
-    <row r="11" ht="15" spans="1:2">
-      <c r="A11" s="4" t="s">
+    <row r="11" customFormat="1" ht="15" spans="1:3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" customFormat="1" ht="30" spans="1:3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C12" s="9" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="4"/>
-      <c r="B12" t="s">
+    <row r="13" customFormat="1" ht="15" spans="1:3">
+      <c r="A13" s="4"/>
+      <c r="B13" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="13" ht="15" spans="1:2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" customFormat="1" ht="15" spans="1:3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" customFormat="1" ht="30" spans="1:3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="8" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="14" ht="15" spans="1:2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5" t="s">
+      <c r="C15" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" customFormat="1" spans="1:2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="8" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="15" ht="15" spans="1:2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5" t="s">
+    <row r="17" customFormat="1" spans="1:2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="8" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="16" ht="15" spans="1:2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5" t="s">
+    <row r="18" customFormat="1" spans="1:2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="8" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="17" ht="15" spans="1:2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="18" ht="15" spans="1:2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+    <row r="19" customFormat="1" ht="18" spans="1:2">
       <c r="A19" s="4"/>
-      <c r="B19" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="20" ht="15" spans="1:2">
+      <c r="B19" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" customFormat="1" ht="18" spans="1:2">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="21" customFormat="1" ht="15" spans="1:3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" customFormat="1" ht="18" spans="1:2">
       <c r="A21" s="4"/>
-      <c r="B21" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="7"/>
-    </row>
-    <row r="22" customFormat="1" ht="30" spans="1:3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="8" t="s">
+      <c r="B21" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" customFormat="1" spans="1:2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23" ht="24.75" spans="1:2">
+      <c r="A23" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" customFormat="1" ht="15" spans="1:2">
+      <c r="A24" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="B24" s="5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="23" customFormat="1" ht="15" spans="1:3">
-      <c r="A23" s="4"/>
-      <c r="B23" t="s">
+    <row r="25" customFormat="1" ht="15" spans="1:2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C23" s="7"/>
-    </row>
-    <row r="24" customFormat="1" ht="15" spans="1:3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="7"/>
-    </row>
-    <row r="25" customFormat="1" ht="30" spans="1:3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="8" t="s">
+    </row>
+    <row r="26" customFormat="1" ht="15" spans="1:2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="26" customFormat="1" spans="1:2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="8" t="s">
+    </row>
+    <row r="27" customFormat="1" ht="15" spans="1:2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="27" customFormat="1" spans="1:2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="8" t="s">
+    <row r="28" customFormat="1" ht="15" spans="1:2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="28" customFormat="1" spans="1:2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="8" t="s">
+    <row r="29" customFormat="1" ht="15" spans="1:2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="11" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="29" customFormat="1" spans="1:2">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-    </row>
-    <row r="30" ht="24.75" spans="1:2">
-      <c r="A30" s="3" t="s">
+    <row r="30" customFormat="1" ht="15" spans="1:2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="B30" s="3"/>
     </row>
     <row r="31" customFormat="1" ht="15" spans="1:2">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="4"/>
+      <c r="B31" s="11" t="s">
         <v>175</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="32" customFormat="1" ht="15" spans="1:2">
       <c r="A32" s="4"/>
       <c r="B32" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" customFormat="1" ht="15" spans="1:2">
       <c r="A33" s="4"/>
       <c r="B33" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" ht="11" customHeight="1"/>
+    <row r="35" ht="15" spans="1:2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" ht="30" spans="1:3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="12" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="34" customFormat="1" ht="15" spans="1:2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5" t="s">
+      <c r="C36" s="9" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="35" customFormat="1" ht="15" spans="1:2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5" t="s">
+    <row r="37" ht="15" spans="1:2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" ht="30" spans="1:3">
+      <c r="A38" s="4"/>
+      <c r="B38" s="12" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="36" customFormat="1" ht="15" spans="1:2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="11" t="s">
+      <c r="C38" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="4"/>
+      <c r="B39" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="37" customFormat="1" ht="15" spans="1:2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="11" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="12" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="38" customFormat="1" ht="15" spans="1:2">
-      <c r="A38" s="4"/>
-      <c r="B38" s="11" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+    </row>
+    <row r="42" ht="24.75" spans="1:2">
+      <c r="A42" s="3" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="39" customFormat="1" ht="15" spans="1:2">
-      <c r="A39" s="4"/>
-      <c r="B39" s="5" t="s">
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" ht="15" spans="1:2">
+      <c r="A43" s="4" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="40" customFormat="1" ht="15" spans="1:2">
-      <c r="A40" s="4"/>
-      <c r="B40" s="5" t="s">
+      <c r="B43" s="5" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="41" customFormat="1" spans="1:1">
-      <c r="A41" s="4"/>
-    </row>
-    <row r="42" ht="11" customHeight="1"/>
-    <row r="43" customFormat="1" ht="15" spans="1:2">
-      <c r="A43" s="4" t="s">
+    <row r="44" spans="1:2">
+      <c r="A44" s="4"/>
+      <c r="B44" t="s">
         <v>186</v>
       </c>
-      <c r="B43" s="5" t="s">
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="13" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="44" customFormat="1" ht="15" spans="1:2">
-      <c r="A44" s="4"/>
-      <c r="B44" s="5" t="s">
+    <row r="46" ht="15" spans="1:2">
+      <c r="A46" s="4"/>
+      <c r="B46" s="11" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="45" customFormat="1" ht="15" spans="1:2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="46" customFormat="1" ht="15" spans="1:2">
-      <c r="A46" s="4"/>
-      <c r="B46" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="47" customFormat="1" ht="15" spans="1:2">
+    <row r="47" ht="15" spans="1:2">
       <c r="A47" s="4"/>
       <c r="B47" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="48" customFormat="1" ht="15" spans="1:2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" ht="15" spans="1:2">
       <c r="A48" s="4"/>
       <c r="B48" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="49" customFormat="1" ht="15" spans="1:2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" ht="15" spans="1:2">
       <c r="A49" s="4"/>
       <c r="B49" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" ht="15" spans="1:2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" ht="30" spans="1:3">
+      <c r="A52" s="4"/>
+      <c r="B52" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="50" ht="15" spans="1:2">
-      <c r="A50" s="4"/>
-      <c r="B50" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" ht="30" spans="1:3">
-      <c r="A51" s="4"/>
-      <c r="B51" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="52" ht="15" spans="1:2">
-      <c r="A52" s="4"/>
-      <c r="B52" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" ht="30" spans="1:3">
+    <row r="53" spans="1:2">
       <c r="A53" s="4"/>
       <c r="B53" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" ht="15" spans="1:2">
       <c r="A54" s="4"/>
-      <c r="B54" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="B54" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" ht="30" spans="1:3">
       <c r="A55" s="4"/>
       <c r="B55" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="4"/>
+      <c r="B56" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="4"/>
+      <c r="B57" s="12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="4"/>
+      <c r="B58" s="12" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-    </row>
-    <row r="57" ht="24.75" spans="1:2">
-      <c r="A57" s="3" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+    </row>
+    <row r="60" ht="24.75" spans="1:2">
+      <c r="A60" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" ht="15" spans="1:2">
-      <c r="A58" s="4" t="s">
+      <c r="B60" s="3"/>
+    </row>
+    <row r="61" ht="15" spans="1:2">
+      <c r="A61" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B61" s="11" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="4"/>
-      <c r="B59" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="4"/>
-      <c r="B60" s="13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="61" ht="15" spans="1:2">
-      <c r="A61" s="4"/>
-      <c r="B61" s="11" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="62" ht="15" spans="1:2">
       <c r="A62" s="4"/>
-      <c r="B62" s="5" t="s">
-        <v>205</v>
+      <c r="B62" s="11" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="63" ht="15" spans="1:2">
       <c r="A63" s="4"/>
-      <c r="B63" s="5" t="s">
-        <v>206</v>
+      <c r="B63" s="11" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="64" ht="15" spans="1:2">
       <c r="A64" s="4"/>
-      <c r="B64" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="4" t="s">
+      <c r="B64" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="65" ht="15" spans="1:2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="66" ht="18" spans="1:1">
+      <c r="A66" s="4"/>
+    </row>
+    <row r="67" ht="15" spans="1:2">
+      <c r="A67" s="4"/>
+      <c r="B67" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" ht="30" spans="1:3">
+      <c r="A68" s="4"/>
+      <c r="B68" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="C68" s="7" t="s">
         <v>207</v>
-      </c>
-      <c r="B66" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="4"/>
-      <c r="B67" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="4"/>
-      <c r="B68" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="4"/>
-      <c r="B69" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="B69" s="12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="70" ht="15" spans="1:2">
       <c r="A70" s="4"/>
-      <c r="B70" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="B70" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" ht="30" spans="1:3">
       <c r="A71" s="4"/>
-      <c r="B71" t="s">
-        <v>212</v>
+      <c r="B71" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="4"/>
-      <c r="B72" t="s">
-        <v>213</v>
+      <c r="B72" s="12" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="4"/>
-      <c r="B73" t="s">
+      <c r="B73" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="74" ht="9" customHeight="1" spans="1:2">
+      <c r="A74" s="10"/>
+      <c r="B74" s="10"/>
+    </row>
+    <row r="75" s="1" customFormat="1" ht="24.75" spans="1:2">
+      <c r="A75" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B75" s="3"/>
+    </row>
+    <row r="76" ht="15" spans="1:2">
+      <c r="A76" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" ht="30" spans="1:3">
+      <c r="A77" s="4"/>
+      <c r="B77" s="12" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="74" ht="18" spans="1:2">
-      <c r="A74" s="4"/>
-      <c r="B74" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="75" ht="30" spans="1:3">
-      <c r="A75" s="4"/>
-      <c r="B75" s="12" t="s">
+      <c r="C77" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="C75" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="76" ht="18" spans="1:2">
-      <c r="A76" s="4"/>
-      <c r="B76" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="77" ht="18" spans="1:2">
-      <c r="A77" s="4"/>
-      <c r="B77" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="78" ht="30" spans="1:3">
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" s="4"/>
       <c r="B78" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="C78" s="7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="79" ht="18" spans="1:2">
+    <row r="79" ht="30" spans="1:3">
       <c r="A79" s="4"/>
       <c r="B79" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="80" ht="18" spans="1:2">
+        <v>217</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="80" ht="15" spans="1:2">
       <c r="A80" s="4"/>
-      <c r="B80" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="81" ht="18" spans="1:2">
+      <c r="B80" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="81" ht="30" spans="1:3">
       <c r="A81" s="4"/>
       <c r="B81" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="4"/>
+      <c r="B82" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="4"/>
+      <c r="B83" s="12" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="10"/>
-      <c r="B82" s="10"/>
-    </row>
-    <row r="83" ht="24.75" spans="1:2">
-      <c r="A83" s="3" t="s">
+    <row r="84" ht="30" spans="1:3">
+      <c r="A84" s="4"/>
+      <c r="B84" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" ht="15" spans="1:2">
-      <c r="A84" s="4" t="s">
+      <c r="C84" s="7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="4"/>
+      <c r="B85" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="B84" s="11" t="s">
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="4"/>
+      <c r="B86" s="12" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="85" ht="15" spans="1:2">
-      <c r="A85" s="4"/>
-      <c r="B85" s="11" t="s">
+    <row r="87" spans="1:2">
+      <c r="A87" s="4"/>
+      <c r="B87" s="12" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="86" ht="15" spans="1:2">
-      <c r="A86" s="4"/>
-      <c r="B86" s="11" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="87" ht="15" spans="1:2">
-      <c r="A87" s="4"/>
-      <c r="B87" s="11" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="88" ht="15" spans="1:2">
-      <c r="A88" s="4"/>
-      <c r="B88" s="11" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="89" ht="18" spans="1:1">
-      <c r="A89" s="4"/>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="B90" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
-      <c r="A91" s="4"/>
-      <c r="B91" t="s">
-        <v>230</v>
-      </c>
-      <c r="E91" s="14"/>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="4"/>
-      <c r="B92" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="4"/>
-      <c r="B93" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="94" ht="18" spans="1:2">
-      <c r="A94" s="4"/>
-      <c r="B94" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="95" ht="30" spans="1:3">
-      <c r="A95" s="4"/>
-      <c r="B95" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="96" ht="18" spans="1:2">
-      <c r="A96" s="4"/>
-      <c r="B96" s="12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="97" ht="18" spans="1:2">
-      <c r="A97" s="4"/>
-      <c r="B97" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="98" ht="30" spans="1:3">
-      <c r="A98" s="4"/>
-      <c r="B98" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="99" ht="18" spans="1:2">
-      <c r="A99" s="4"/>
-      <c r="B99" s="12" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="100" ht="18" spans="1:2">
-      <c r="A100" s="4"/>
-      <c r="B100" s="12" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="101" ht="9" customHeight="1" spans="1:2">
-      <c r="A101" s="10"/>
-      <c r="B101" s="10"/>
-    </row>
-    <row r="102" s="1" customFormat="1" ht="24.75" spans="1:2">
-      <c r="A102" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B102" s="3"/>
-    </row>
-    <row r="103" s="1" customFormat="1" ht="15" spans="1:2">
-      <c r="A103" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="B103" s="11" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="104" s="1" customFormat="1" ht="18" customHeight="1" spans="1:2">
-      <c r="A104" s="4"/>
-      <c r="B104" s="11" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="105" s="1" customFormat="1" ht="15" spans="1:2">
-      <c r="A105" s="4"/>
-      <c r="B105" s="11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="106" s="1" customFormat="1" ht="15" spans="1:2">
-      <c r="A106" s="4"/>
-      <c r="B106" s="11" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="107" ht="15" spans="1:2">
-      <c r="A107" s="4"/>
-      <c r="B107" s="11" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="4"/>
-      <c r="B108" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="109" ht="18" spans="1:2">
-      <c r="A109" s="4"/>
-      <c r="B109" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="110" ht="30" spans="1:3">
-      <c r="A110" s="4"/>
-      <c r="B110" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="C110" s="7" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="111" ht="18" spans="1:2">
-      <c r="A111" s="4"/>
-      <c r="B111" s="12" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="112" ht="30" spans="1:3">
-      <c r="A112" s="4"/>
-      <c r="B112" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="C112" s="7" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="113" ht="18" spans="1:2">
-      <c r="A113" s="4"/>
-      <c r="B113" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="114" ht="30" spans="1:3">
-      <c r="A114" s="4"/>
-      <c r="B114" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="C114" s="7" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="115" ht="18" spans="1:2">
-      <c r="A115" s="4"/>
-      <c r="B115" s="12" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="116" ht="18" spans="1:2">
-      <c r="A116" s="4"/>
-      <c r="B116" s="12" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="117" ht="30" spans="1:3">
-      <c r="A117" s="4"/>
-      <c r="B117" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="C117" s="7" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="118" ht="18" spans="1:2">
-      <c r="A118" s="4"/>
-      <c r="B118" s="12" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="119" ht="18" spans="1:2">
-      <c r="A119" s="4"/>
-      <c r="B119" s="12" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="120" ht="18" spans="1:2">
-      <c r="A120" s="4"/>
-      <c r="B120" s="12" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="A121" s="10"/>
-      <c r="B121" s="10"/>
+    <row r="88" spans="1:2">
+      <c r="A88" s="10"/>
+      <c r="B88" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A75:B75"/>
     <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A11:A28"/>
-    <mergeCell ref="A31:A41"/>
-    <mergeCell ref="A43:A55"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A66:A73"/>
-    <mergeCell ref="A84:A88"/>
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="A103:A108"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A24:A33"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="A43:A49"/>
+    <mergeCell ref="A51:A58"/>
+    <mergeCell ref="A61:A65"/>
+    <mergeCell ref="A67:A73"/>
+    <mergeCell ref="A76:A87"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C22" r:id="rId1" display="https://www.hackerrank.com/interview/interview-preparation-kit/search/challenges"/>
-    <hyperlink ref="C25" r:id="rId1" display="https://www.hackerrank.com/interview/interview-preparation-kit/search/challenges"/>
-    <hyperlink ref="C51" r:id="rId2" display="https://www.hackerrank.com/interview/interview-preparation-kit/dynamic-programming/challenges"/>
-    <hyperlink ref="C53" r:id="rId2" display="https://www.hackerrank.com/interview/interview-preparation-kit/dynamic-programming/challenges"/>
-    <hyperlink ref="C75" r:id="rId3" display="https://www.hackerrank.com/interview/interview-preparation-kit/stacks-queues/challenges"/>
-    <hyperlink ref="C78" r:id="rId3" display="https://www.hackerrank.com/interview/interview-preparation-kit/stacks-queues/challenges"/>
-    <hyperlink ref="C95" r:id="rId4" display="https://www.hackerrank.com/interview/interview-preparation-kit/graphs/challenges"/>
-    <hyperlink ref="C98" r:id="rId4" display="https://www.hackerrank.com/interview/interview-preparation-kit/graphs/challenges"/>
-    <hyperlink ref="C110" r:id="rId5" display="https://www.hackerrank.com/interview/interview-preparation-kit/trees/challenges"/>
-    <hyperlink ref="C112" r:id="rId6" display="https://www.hackerrank.com/interview/interview-preparation-kit/linked-lists/challenges"/>
-    <hyperlink ref="C117" r:id="rId6" display="https://www.hackerrank.com/interview/interview-preparation-kit/linked-lists/challenges"/>
-    <hyperlink ref="C114" r:id="rId5" display="https://www.hackerrank.com/interview/interview-preparation-kit/trees/challenges"/>
+    <hyperlink ref="C12" r:id="rId1" display="https://www.hackerrank.com/interview/interview-preparation-kit/search/challenges"/>
+    <hyperlink ref="C15" r:id="rId1" display="https://www.hackerrank.com/interview/interview-preparation-kit/search/challenges"/>
+    <hyperlink ref="C36" r:id="rId2" display="https://www.hackerrank.com/interview/interview-preparation-kit/dynamic-programming/challenges"/>
+    <hyperlink ref="C38" r:id="rId2" display="https://www.hackerrank.com/interview/interview-preparation-kit/dynamic-programming/challenges"/>
+    <hyperlink ref="C52" r:id="rId3" display="https://www.hackerrank.com/interview/interview-preparation-kit/stacks-queues/challenges"/>
+    <hyperlink ref="C55" r:id="rId3" display="https://www.hackerrank.com/interview/interview-preparation-kit/stacks-queues/challenges"/>
+    <hyperlink ref="C68" r:id="rId4" display="https://www.hackerrank.com/interview/interview-preparation-kit/graphs/challenges"/>
+    <hyperlink ref="C71" r:id="rId4" display="https://www.hackerrank.com/interview/interview-preparation-kit/graphs/challenges"/>
+    <hyperlink ref="C77" r:id="rId5" display="https://www.hackerrank.com/interview/interview-preparation-kit/trees/challenges"/>
+    <hyperlink ref="C79" r:id="rId6" display="https://www.hackerrank.com/interview/interview-preparation-kit/linked-lists/challenges"/>
+    <hyperlink ref="C84" r:id="rId6" display="https://www.hackerrank.com/interview/interview-preparation-kit/linked-lists/challenges"/>
+    <hyperlink ref="C81" r:id="rId5" display="https://www.hackerrank.com/interview/interview-preparation-kit/trees/challenges"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Added Hands On and HackerRank Demos - Day 5 and 6.
</commit_message>
<xml_diff>
--- a/Java 8 & 11 - TOC.xlsx
+++ b/Java 8 & 11 - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="2"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -701,10 +701,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -792,10 +792,41 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -808,7 +839,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -830,23 +869,22 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -860,35 +898,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -899,22 +912,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -947,7 +947,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -959,19 +1001,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -983,31 +1031,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1019,25 +1061,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1049,85 +1121,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1208,6 +1208,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1219,15 +1228,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1249,11 +1249,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1273,30 +1286,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1305,18 +1294,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1329,131 +1329,131 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1507,6 +1507,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1873,56 +1876,56 @@
   <sheetData>
     <row r="7" ht="13.5"/>
     <row r="8" ht="13.5" spans="6:9">
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="6:9">
-      <c r="F9" s="24">
+      <c r="F9" s="25">
         <v>1</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="27">
         <v>5</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="27">
         <v>20</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="6:9">
-      <c r="F10" s="27">
+      <c r="F10" s="28">
         <v>2</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="27">
         <v>5</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10" s="27">
         <v>20</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="6:9">
-      <c r="F11" s="29"/>
-      <c r="G11" s="30" t="s">
+      <c r="F11" s="30"/>
+      <c r="G11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="32" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1937,10 +1940,10 @@
   <sheetPr/>
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C141" sqref="C141"/>
+      <selection pane="bottomLeft" activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -1948,6 +1951,7 @@
     <col min="1" max="1" width="35.125" customWidth="1"/>
     <col min="2" max="2" width="43.75" customWidth="1"/>
     <col min="3" max="3" width="45.625" customWidth="1"/>
+    <col min="4" max="4" width="18.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" spans="1:3">
@@ -2782,10 +2786,10 @@
     </row>
     <row r="131" ht="30" spans="1:3">
       <c r="A131" s="4"/>
-      <c r="B131" s="11" t="s">
+      <c r="B131" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="C131" s="7" t="s">
+      <c r="C131" s="9" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2897,10 +2901,10 @@
   <sheetPr/>
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
Added HackerRank Assessments - Day 7.
</commit_message>
<xml_diff>
--- a/Java 8 & 11 - TOC.xlsx
+++ b/Java 8 & 11 - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="228">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -519,7 +519,97 @@
     <t>Day 7</t>
   </si>
   <si>
-    <t>3. Language and Library Improvements</t>
+    <t xml:space="preserve">2. Deprecations and Removals </t>
+  </si>
+  <si>
+    <t>1. Removed Methods</t>
+  </si>
+  <si>
+    <t>2. Removed Enterprise APIs</t>
+  </si>
+  <si>
+    <t>3. JavaFX Moving to OpenJFX</t>
+  </si>
+  <si>
+    <t>4. Removed &amp; Deprecated Technologies</t>
+  </si>
+  <si>
+    <t>5. Summary</t>
+  </si>
+  <si>
+    <t>Max Array Sum</t>
+  </si>
+  <si>
+    <t>https://www.hackerrank.com/interview/interview-preparation-kit/dynamic-programming/challenges</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>Candies</t>
+  </si>
+  <si>
+    <t>Decibinary Numbers</t>
+  </si>
+  <si>
+    <t>Circular Printer</t>
+  </si>
+  <si>
+    <t>Maximizing the Final Element</t>
+  </si>
+  <si>
+    <t>Day 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.  Performance and Security Improvements </t>
+  </si>
+  <si>
+    <t>1. Garbage Collection Improvements</t>
+  </si>
+  <si>
+    <t>2. Epsilon: A No-Op Garbage Collector</t>
+  </si>
+  <si>
+    <t>3. Improved Aarch64 Intrinsics</t>
+  </si>
+  <si>
+    <t>4.  Flight Recorder</t>
+  </si>
+  <si>
+    <t>5.  Dynamic Class-File Constants</t>
+  </si>
+  <si>
+    <t>6. Security Improvement: TLS 1.3</t>
+  </si>
+  <si>
+    <t>7. Summary</t>
+  </si>
+  <si>
+    <t>Balanced Brackets</t>
+  </si>
+  <si>
+    <t>https://www.hackerrank.com/interview/interview-preparation-kit/stacks-queues/challenges</t>
+  </si>
+  <si>
+    <t>Queues: A Tale of Two Stacks</t>
+  </si>
+  <si>
+    <t>Largest Rectangle</t>
+  </si>
+  <si>
+    <t>Min Max Riddle</t>
+  </si>
+  <si>
+    <t>Castle on the Grid</t>
+  </si>
+  <si>
+    <t>Poisonous Plants</t>
+  </si>
+  <si>
+    <t>Day 9</t>
+  </si>
+  <si>
+    <t>4. Language and Library Improvements</t>
   </si>
   <si>
     <t>1. HttpClient API</t>
@@ -552,90 +642,6 @@
     <t>10.Summary</t>
   </si>
   <si>
-    <t>Max Array Sum</t>
-  </si>
-  <si>
-    <t>https://www.hackerrank.com/interview/interview-preparation-kit/dynamic-programming/challenges</t>
-  </si>
-  <si>
-    <t>Abbreviation</t>
-  </si>
-  <si>
-    <t>Candies</t>
-  </si>
-  <si>
-    <t>Decibinary Numbers</t>
-  </si>
-  <si>
-    <t>Day 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.  Performance and Security Improvements </t>
-  </si>
-  <si>
-    <t>1. Garbage Collection Improvements</t>
-  </si>
-  <si>
-    <t>2. Epsilon: A No-Op Garbage Collector</t>
-  </si>
-  <si>
-    <t>3. Improved Aarch64 Intrinsics</t>
-  </si>
-  <si>
-    <t>4.  Flight Recorder</t>
-  </si>
-  <si>
-    <t>5.  Dynamic Class-File Constants</t>
-  </si>
-  <si>
-    <t>6. Security Improvement: TLS 1.3</t>
-  </si>
-  <si>
-    <t>7. Summary</t>
-  </si>
-  <si>
-    <t>Balanced Brackets</t>
-  </si>
-  <si>
-    <t>https://www.hackerrank.com/interview/interview-preparation-kit/stacks-queues/challenges</t>
-  </si>
-  <si>
-    <t>Queues: A Tale of Two Stacks</t>
-  </si>
-  <si>
-    <t>Largest Rectangle</t>
-  </si>
-  <si>
-    <t>Min Max Riddle</t>
-  </si>
-  <si>
-    <t>Castle on the Grid</t>
-  </si>
-  <si>
-    <t>Poisonous Plants</t>
-  </si>
-  <si>
-    <t>Day 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7. Deprecations and Removals </t>
-  </si>
-  <si>
-    <t>1. Removed Methods</t>
-  </si>
-  <si>
-    <t>2. Removed Enterprise APIs</t>
-  </si>
-  <si>
-    <t>3. JavaFX Moving to OpenJFX</t>
-  </si>
-  <si>
-    <t>4. Removed &amp; Deprecated Technologies</t>
-  </si>
-  <si>
-    <t>5. Summary</t>
-  </si>
-  <si>
     <t>Roads and Libraries</t>
   </si>
   <si>
@@ -657,7 +663,7 @@
     <t>Day 10</t>
   </si>
   <si>
-    <t>Hands On Demos</t>
+    <t>5. Hands On Demos</t>
   </si>
   <si>
     <t>Tree: Height of a Binary Tree</t>
@@ -701,10 +707,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -792,11 +798,17 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -808,7 +820,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -823,44 +867,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -870,7 +876,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -878,6 +884,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -906,15 +920,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -947,12 +953,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -971,13 +971,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -995,13 +995,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1019,103 +1103,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1127,7 +1121,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1208,15 +1214,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1228,6 +1225,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1256,17 +1262,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1286,6 +1288,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1294,21 +1311,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1329,37 +1335,37 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1368,88 +1374,88 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1940,8 +1946,8 @@
   <sheetPr/>
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C134" sqref="C134"/>
     </sheetView>
@@ -2899,12 +2905,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20:B21"/>
+      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -3065,438 +3071,471 @@
       <c r="A24" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="11" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="25" customFormat="1" ht="15" spans="1:2">
       <c r="A25" s="4"/>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="26" customFormat="1" ht="15" spans="1:2">
       <c r="A26" s="4"/>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="11" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="27" customFormat="1" ht="15" spans="1:2">
       <c r="A27" s="4"/>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="11" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="28" customFormat="1" ht="15" spans="1:2">
       <c r="A28" s="4"/>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="29" customFormat="1" ht="15" spans="1:2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="11" t="s">
+    <row r="29" ht="11" customHeight="1"/>
+    <row r="30" ht="15" spans="1:2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" ht="30" spans="1:3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="12" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="30" customFormat="1" ht="15" spans="1:2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="11" t="s">
+      <c r="C31" s="9" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="31" customFormat="1" ht="15" spans="1:2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="11" t="s">
+    <row r="32" ht="15" spans="1:2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" ht="30" spans="1:3">
+      <c r="A33" s="4"/>
+      <c r="B33" s="12" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="32" customFormat="1" ht="15" spans="1:2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5" t="s">
+      <c r="C33" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="4"/>
+      <c r="B34" s="12" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="33" customFormat="1" ht="15" spans="1:2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="12" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="34" ht="11" customHeight="1"/>
-    <row r="35" ht="15" spans="1:2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" ht="30" spans="1:3">
+    <row r="36" ht="18" spans="1:2">
       <c r="A36" s="4"/>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" ht="18" spans="1:2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C36" s="9" t="s">
+    </row>
+    <row r="38" ht="18" spans="1:2">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="37" ht="15" spans="1:2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" ht="30" spans="1:3">
-      <c r="A38" s="4"/>
-      <c r="B38" s="12" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+    </row>
+    <row r="40" ht="24.75" spans="1:2">
+      <c r="A40" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="4"/>
-      <c r="B39" s="12" t="s">
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" ht="15" spans="1:2">
+      <c r="A41" s="4" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="4"/>
-      <c r="B40" s="12" t="s">
+      <c r="B41" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-    </row>
-    <row r="42" ht="24.75" spans="1:2">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="4"/>
+      <c r="B42" t="s">
         <v>183</v>
       </c>
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" ht="15" spans="1:2">
-      <c r="A43" s="4" t="s">
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="4"/>
+      <c r="B43" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="B43" s="5" t="s">
+    </row>
+    <row r="44" ht="15" spans="1:2">
+      <c r="A44" s="4"/>
+      <c r="B44" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="4"/>
-      <c r="B44" t="s">
+    <row r="45" ht="15" spans="1:2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="5" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="13" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="46" ht="15" spans="1:2">
       <c r="A46" s="4"/>
-      <c r="B46" s="11" t="s">
-        <v>188</v>
+      <c r="B46" s="5" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="47" ht="15" spans="1:2">
       <c r="A47" s="4"/>
       <c r="B47" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="48" ht="15" spans="1:2">
-      <c r="A48" s="4"/>
-      <c r="B48" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:2">
       <c r="A49" s="4"/>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" ht="30" spans="1:3">
+      <c r="A50" s="4"/>
+      <c r="B50" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="12" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="51" ht="15" spans="1:2">
-      <c r="A51" s="4"/>
-      <c r="B51" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" ht="30" spans="1:3">
+    <row r="52" ht="15" spans="1:2">
       <c r="A52" s="4"/>
-      <c r="B52" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="B52" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" ht="30" spans="1:3">
       <c r="A53" s="4"/>
       <c r="B53" s="12" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="54" ht="15" spans="1:2">
+        <v>192</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" s="4"/>
-      <c r="B54" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" ht="30" spans="1:3">
+      <c r="B54" s="12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" s="4"/>
       <c r="B55" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="4"/>
       <c r="B56" s="12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="57" ht="18" spans="1:2">
+      <c r="A57" s="4"/>
+      <c r="B57" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" ht="18" spans="1:2">
+      <c r="A58" s="4"/>
+      <c r="B58" s="5"/>
+    </row>
+    <row r="59" ht="18" spans="1:2">
+      <c r="A59" s="4"/>
+      <c r="B59" s="5"/>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
+    </row>
+    <row r="61" ht="24.75" spans="1:2">
+      <c r="A61" s="3" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="4"/>
-      <c r="B57" s="12" t="s">
+      <c r="B61" s="3"/>
+    </row>
+    <row r="62" customFormat="1" ht="15" spans="1:2">
+      <c r="A62" s="4" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="4"/>
-      <c r="B58" s="12" t="s">
+      <c r="B62" s="5" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="10"/>
-      <c r="B59" s="10"/>
-    </row>
-    <row r="60" ht="24.75" spans="1:2">
-      <c r="A60" s="3" t="s">
+    <row r="63" customFormat="1" ht="15" spans="1:2">
+      <c r="A63" s="4"/>
+      <c r="B63" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" ht="15" spans="1:2">
-      <c r="A61" s="4" t="s">
+    </row>
+    <row r="64" customFormat="1" ht="15" spans="1:2">
+      <c r="A64" s="4"/>
+      <c r="B64" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="B61" s="11" t="s">
+    </row>
+    <row r="65" customFormat="1" ht="15" spans="1:2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="62" ht="15" spans="1:2">
-      <c r="A62" s="4"/>
-      <c r="B62" s="11" t="s">
+    <row r="66" customFormat="1" ht="15" spans="1:2">
+      <c r="A66" s="4"/>
+      <c r="B66" s="5" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="63" ht="15" spans="1:2">
-      <c r="A63" s="4"/>
-      <c r="B63" s="11" t="s">
+    <row r="67" customFormat="1" ht="15" spans="1:2">
+      <c r="A67" s="4"/>
+      <c r="B67" s="11" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="64" ht="15" spans="1:2">
-      <c r="A64" s="4"/>
-      <c r="B64" s="11" t="s">
+    <row r="68" customFormat="1" ht="15" spans="1:2">
+      <c r="A68" s="4"/>
+      <c r="B68" s="11" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="65" ht="15" spans="1:2">
-      <c r="A65" s="4"/>
-      <c r="B65" s="11" t="s">
+    <row r="69" customFormat="1" ht="15" spans="1:2">
+      <c r="A69" s="4"/>
+      <c r="B69" s="11" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="66" ht="18" spans="1:1">
-      <c r="A66" s="4"/>
-    </row>
-    <row r="67" ht="15" spans="1:2">
-      <c r="A67" s="4"/>
-      <c r="B67" s="6" t="s">
+    <row r="70" customFormat="1" ht="15" spans="1:2">
+      <c r="A70" s="4"/>
+      <c r="B70" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="71" customFormat="1" ht="15" spans="1:2">
+      <c r="A71" s="4"/>
+      <c r="B71" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="72" customFormat="1" ht="9" customHeight="1" spans="1:2">
+      <c r="A72" s="4"/>
+      <c r="B72" s="5"/>
+    </row>
+    <row r="73" ht="15" spans="1:2">
+      <c r="A73" s="4"/>
+      <c r="B73" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="68" ht="30" spans="1:3">
-      <c r="A68" s="4"/>
-      <c r="B68" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="4"/>
-      <c r="B69" s="12" t="s">
+    <row r="74" ht="30" spans="1:3">
+      <c r="A74" s="4"/>
+      <c r="B74" s="12" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="70" ht="15" spans="1:2">
-      <c r="A70" s="4"/>
-      <c r="B70" s="6" t="s">
+      <c r="C74" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="4"/>
+      <c r="B75" s="12" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="76" ht="15" spans="1:2">
+      <c r="A76" s="4"/>
+      <c r="B76" s="6" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="71" ht="30" spans="1:3">
-      <c r="A71" s="4"/>
-      <c r="B71" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="4"/>
-      <c r="B72" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="4"/>
-      <c r="B73" s="12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="74" ht="9" customHeight="1" spans="1:2">
-      <c r="A74" s="10"/>
-      <c r="B74" s="10"/>
-    </row>
-    <row r="75" s="1" customFormat="1" ht="24.75" spans="1:2">
-      <c r="A75" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="B75" s="3"/>
-    </row>
-    <row r="76" ht="15" spans="1:2">
-      <c r="A76" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="77" ht="30" spans="1:3">
       <c r="A77" s="4"/>
       <c r="B77" s="12" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="4"/>
       <c r="B78" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="79" ht="30" spans="1:3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
       <c r="A79" s="4"/>
       <c r="B79" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="80" ht="15" spans="1:2">
-      <c r="A80" s="4"/>
-      <c r="B80" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="81" ht="30" spans="1:3">
-      <c r="A81" s="4"/>
-      <c r="B81" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="C81" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="80" ht="9" customHeight="1" spans="1:2">
+      <c r="A80" s="10"/>
+      <c r="B80" s="10"/>
+    </row>
+    <row r="81" s="1" customFormat="1" ht="24.75" spans="1:2">
+      <c r="A81" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82" ht="15" spans="1:2">
+      <c r="A82" s="4" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="4"/>
-      <c r="B82" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="B82" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" ht="30" spans="1:3">
       <c r="A83" s="4"/>
       <c r="B83" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="84" ht="30" spans="1:3">
+        <v>216</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84" s="4"/>
       <c r="B84" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="C84" s="7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" ht="30" spans="1:3">
       <c r="A85" s="4"/>
       <c r="B85" s="12" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
+        <v>219</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="86" ht="15" spans="1:2">
       <c r="A86" s="4"/>
-      <c r="B86" s="12" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="B86" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="87" ht="30" spans="1:3">
       <c r="A87" s="4"/>
       <c r="B87" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="4"/>
+      <c r="B88" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="4"/>
+      <c r="B89" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="90" ht="30" spans="1:3">
+      <c r="A90" s="4"/>
+      <c r="B90" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="4"/>
+      <c r="B91" s="12" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="10"/>
-      <c r="B88" s="10"/>
+    <row r="92" spans="1:2">
+      <c r="A92" s="4"/>
+      <c r="B92" s="12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="4"/>
+      <c r="B93" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="10"/>
+      <c r="B94" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A81:B81"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A24:A33"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="A43:A49"/>
-    <mergeCell ref="A51:A58"/>
-    <mergeCell ref="A61:A65"/>
-    <mergeCell ref="A67:A73"/>
-    <mergeCell ref="A76:A87"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A62:A71"/>
+    <mergeCell ref="A73:A79"/>
+    <mergeCell ref="A82:A93"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1" display="https://www.hackerrank.com/interview/interview-preparation-kit/search/challenges"/>
     <hyperlink ref="C15" r:id="rId1" display="https://www.hackerrank.com/interview/interview-preparation-kit/search/challenges"/>
-    <hyperlink ref="C36" r:id="rId2" display="https://www.hackerrank.com/interview/interview-preparation-kit/dynamic-programming/challenges"/>
-    <hyperlink ref="C38" r:id="rId2" display="https://www.hackerrank.com/interview/interview-preparation-kit/dynamic-programming/challenges"/>
-    <hyperlink ref="C52" r:id="rId3" display="https://www.hackerrank.com/interview/interview-preparation-kit/stacks-queues/challenges"/>
-    <hyperlink ref="C55" r:id="rId3" display="https://www.hackerrank.com/interview/interview-preparation-kit/stacks-queues/challenges"/>
-    <hyperlink ref="C68" r:id="rId4" display="https://www.hackerrank.com/interview/interview-preparation-kit/graphs/challenges"/>
-    <hyperlink ref="C71" r:id="rId4" display="https://www.hackerrank.com/interview/interview-preparation-kit/graphs/challenges"/>
-    <hyperlink ref="C77" r:id="rId5" display="https://www.hackerrank.com/interview/interview-preparation-kit/trees/challenges"/>
-    <hyperlink ref="C79" r:id="rId6" display="https://www.hackerrank.com/interview/interview-preparation-kit/linked-lists/challenges"/>
-    <hyperlink ref="C84" r:id="rId6" display="https://www.hackerrank.com/interview/interview-preparation-kit/linked-lists/challenges"/>
-    <hyperlink ref="C81" r:id="rId5" display="https://www.hackerrank.com/interview/interview-preparation-kit/trees/challenges"/>
+    <hyperlink ref="C31" r:id="rId2" display="https://www.hackerrank.com/interview/interview-preparation-kit/dynamic-programming/challenges"/>
+    <hyperlink ref="C33" r:id="rId2" display="https://www.hackerrank.com/interview/interview-preparation-kit/dynamic-programming/challenges"/>
+    <hyperlink ref="C50" r:id="rId3" display="https://www.hackerrank.com/interview/interview-preparation-kit/stacks-queues/challenges"/>
+    <hyperlink ref="C53" r:id="rId3" display="https://www.hackerrank.com/interview/interview-preparation-kit/stacks-queues/challenges"/>
+    <hyperlink ref="C74" r:id="rId4" display="https://www.hackerrank.com/interview/interview-preparation-kit/graphs/challenges"/>
+    <hyperlink ref="C77" r:id="rId4" display="https://www.hackerrank.com/interview/interview-preparation-kit/graphs/challenges"/>
+    <hyperlink ref="C83" r:id="rId5" display="https://www.hackerrank.com/interview/interview-preparation-kit/trees/challenges"/>
+    <hyperlink ref="C85" r:id="rId6" display="https://www.hackerrank.com/interview/interview-preparation-kit/linked-lists/challenges"/>
+    <hyperlink ref="C90" r:id="rId6" display="https://www.hackerrank.com/interview/interview-preparation-kit/linked-lists/challenges"/>
+    <hyperlink ref="C87" r:id="rId5" display="https://www.hackerrank.com/interview/interview-preparation-kit/trees/challenges"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Added HackerRank Assessments - Day 8.
</commit_message>
<xml_diff>
--- a/Java 8 & 11 - TOC.xlsx
+++ b/Java 8 & 11 - TOC.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="230">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -604,6 +604,12 @@
   </si>
   <si>
     <t>Poisonous Plants</t>
+  </si>
+  <si>
+    <t>Character Reprogramming</t>
+  </si>
+  <si>
+    <t>Featured Products</t>
   </si>
   <si>
     <t>Day 9</t>
@@ -707,10 +713,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -805,8 +811,85 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -821,84 +904,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -913,14 +919,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -953,13 +959,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -971,7 +971,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -983,13 +989,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1007,7 +1013,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1019,55 +1067,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1079,31 +1091,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1127,13 +1115,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1216,10 +1222,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1240,15 +1244,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1260,30 +1255,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1306,6 +1277,41 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -1314,15 +1320,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1341,121 +1347,121 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2914,9 +2920,9 @@
   <dimension ref="A1:C94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B75" sqref="B75"/>
+      <selection pane="bottomLeft" activeCell="B57" sqref="B57:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -3282,11 +3288,15 @@
     </row>
     <row r="58" ht="18" spans="1:2">
       <c r="A58" s="4"/>
-      <c r="B58" s="5"/>
+      <c r="B58" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="59" ht="18" spans="1:2">
       <c r="A59" s="4"/>
-      <c r="B59" s="5"/>
+      <c r="B59" s="5" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="11"/>
@@ -3294,70 +3304,70 @@
     </row>
     <row r="61" ht="24.75" spans="1:2">
       <c r="A61" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B61" s="3"/>
     </row>
     <row r="62" customFormat="1" ht="15" spans="1:2">
       <c r="A62" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="63" customFormat="1" ht="15" spans="1:2">
       <c r="A63" s="4"/>
       <c r="B63" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="64" customFormat="1" ht="15" spans="1:2">
       <c r="A64" s="4"/>
       <c r="B64" s="5" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="65" customFormat="1" ht="15" spans="1:2">
       <c r="A65" s="4"/>
       <c r="B65" s="5" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="66" customFormat="1" ht="15" spans="1:2">
       <c r="A66" s="4"/>
       <c r="B66" s="5" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" customFormat="1" ht="15" spans="1:2">
       <c r="A67" s="4"/>
       <c r="B67" s="12" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="68" customFormat="1" ht="15" spans="1:2">
       <c r="A68" s="4"/>
       <c r="B68" s="12" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="69" customFormat="1" ht="15" spans="1:2">
       <c r="A69" s="4"/>
       <c r="B69" s="12" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" customFormat="1" ht="15" spans="1:2">
       <c r="A70" s="4"/>
       <c r="B70" s="5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="71" customFormat="1" ht="15" spans="1:2">
       <c r="A71" s="4"/>
       <c r="B71" s="5" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="72" customFormat="1" ht="9" customHeight="1" spans="1:2">
@@ -3373,16 +3383,16 @@
     <row r="74" ht="30" spans="1:3">
       <c r="A74" s="4"/>
       <c r="B74" s="14" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="4"/>
       <c r="B75" s="14" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="76" ht="15" spans="1:2">
@@ -3394,22 +3404,22 @@
     <row r="77" ht="30" spans="1:3">
       <c r="A77" s="4"/>
       <c r="B77" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="C77" s="7" t="s">
         <v>211</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="4"/>
       <c r="B78" s="14" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="4"/>
       <c r="B79" s="14" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="80" ht="9" customHeight="1" spans="1:2">
@@ -3418,13 +3428,13 @@
     </row>
     <row r="81" s="1" customFormat="1" ht="24.75" spans="1:2">
       <c r="A81" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B81" s="3"/>
     </row>
     <row r="82" ht="15" spans="1:2">
       <c r="A82" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>64</v>
@@ -3433,25 +3443,25 @@
     <row r="83" ht="30" spans="1:3">
       <c r="A83" s="4"/>
       <c r="B83" s="14" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="4"/>
       <c r="B84" s="14" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="85" ht="30" spans="1:3">
       <c r="A85" s="4"/>
       <c r="B85" s="14" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="86" ht="15" spans="1:2">
@@ -3463,49 +3473,49 @@
     <row r="87" ht="30" spans="1:3">
       <c r="A87" s="4"/>
       <c r="B87" s="14" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="4"/>
       <c r="B88" s="14" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="4"/>
       <c r="B89" s="14" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="90" ht="30" spans="1:3">
       <c r="A90" s="4"/>
       <c r="B90" s="14" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="4"/>
       <c r="B91" s="14" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="4"/>
       <c r="B92" s="14" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="4"/>
       <c r="B93" s="14" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="94" spans="1:2">

</xml_diff>

<commit_message>
Updated - Day 5.
</commit_message>
<xml_diff>
--- a/Java 8 & 11 - TOC.xlsx
+++ b/Java 8 & 11 - TOC.xlsx
@@ -758,10 +758,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -849,9 +849,23 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -864,38 +878,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -915,19 +902,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -939,6 +917,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -954,19 +955,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1004,6 +1004,126 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1016,115 +1136,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1142,25 +1160,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1172,19 +1178,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1265,17 +1265,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1295,41 +1304,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1339,11 +1313,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1362,18 +1342,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1386,127 +1386,127 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2004,9 +2004,9 @@
   <dimension ref="A1:E142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A96" sqref="$A96:$XFD96"/>
+      <selection pane="bottomLeft" activeCell="B140" sqref="B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -2885,7 +2885,7 @@
       <c r="B136" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="C136" s="7" t="s">
+      <c r="C136" s="9" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2965,9 +2965,9 @@
   <dimension ref="A1:C111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F103" sqref="F103"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -3581,19 +3581,19 @@
         <v>231</v>
       </c>
     </row>
-    <row r="97" ht="18" spans="1:2">
+    <row r="97" ht="15" spans="1:2">
       <c r="A97" s="4"/>
       <c r="B97" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="98" ht="18" spans="1:2">
+    <row r="98" spans="1:2">
       <c r="A98" s="4"/>
       <c r="B98" s="15" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="99" ht="18" spans="1:2">
+    <row r="99" spans="1:2">
       <c r="A99" s="4"/>
       <c r="B99" s="15" t="s">
         <v>233</v>

</xml_diff>

<commit_message>
Updated - Day 5,6 and 9.
</commit_message>
<xml_diff>
--- a/Java 8 & 11 - TOC.xlsx
+++ b/Java 8 & 11 - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -759,9 +759,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -850,7 +850,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -858,37 +858,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -925,8 +902,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -939,9 +933,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -962,6 +955,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -971,7 +971,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1004,19 +1004,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1028,85 +1088,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1118,37 +1124,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1166,7 +1142,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1178,13 +1166,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1265,15 +1265,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1285,6 +1276,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1365,15 +1365,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1386,127 +1386,127 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2003,10 +2003,10 @@
   <sheetPr/>
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B140" sqref="B140"/>
+      <selection pane="bottomLeft" activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -2909,13 +2909,13 @@
     </row>
     <row r="140" ht="18" spans="1:2">
       <c r="A140" s="4"/>
-      <c r="B140" s="5" t="s">
+      <c r="B140" s="12" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="141" ht="18" spans="1:2">
       <c r="A141" s="4"/>
-      <c r="B141" s="5" t="s">
+      <c r="B141" s="12" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2964,8 +2964,8 @@
   <sheetPr/>
   <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>

</xml_diff>

<commit_message>
Updated - Hands On Demos and Assignments and HackerRank Assessments for Further Practice.
</commit_message>
<xml_diff>
--- a/Java 8 & 11 - TOC.xlsx
+++ b/Java 8 & 11 - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="2"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -758,10 +758,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -850,7 +850,59 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -864,13 +916,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -879,15 +924,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -903,14 +941,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -920,7 +950,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -934,37 +964,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1004,7 +1004,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1016,7 +1022,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1028,13 +1088,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1046,7 +1118,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1058,67 +1154,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1130,31 +1166,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1166,25 +1178,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1265,6 +1265,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1314,21 +1340,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1351,21 +1362,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1386,127 +1386,127 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2003,10 +2003,10 @@
   <sheetPr/>
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C147" sqref="C147"/>
+      <selection pane="bottomLeft" activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -2590,7 +2590,7 @@
     </row>
     <row r="89" ht="18" spans="1:2">
       <c r="A89" s="4"/>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="12" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2964,10 +2964,10 @@
   <sheetPr/>
   <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -3104,7 +3104,7 @@
     </row>
     <row r="20" customFormat="1" ht="18" spans="1:2">
       <c r="A20" s="4"/>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="12" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3207,13 +3207,13 @@
     </row>
     <row r="37" ht="18" spans="1:2">
       <c r="A37" s="4"/>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="12" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="38" ht="18" spans="1:2">
       <c r="A38" s="4"/>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="12" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3300,7 +3300,7 @@
       <c r="B53" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="9" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>